<commit_message>
Update vehicle subsidies with latest foreign entities of concern guidance
</commit_message>
<xml_diff>
--- a/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
+++ b/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D670C6-7E61-42B5-9A27-DB763317D586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDA6C5A-A488-4546-90F0-F5782A95BD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="730" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="88">
   <si>
     <t>Sources:</t>
   </si>
@@ -303,7 +303,13 @@
     <t>values from original IRA analysis</t>
   </si>
   <si>
-    <t>values assuming a 75% cut in our original analysis to represent FEOC restrictions</t>
+    <t>values assuming a 56% cut in our original analysis to represent FEOC restrictions</t>
+  </si>
+  <si>
+    <t>Foreign Entities of Concern Multiplier</t>
+  </si>
+  <si>
+    <t>BloombergNEF, MarkLines, Department of Energy</t>
   </si>
 </sst>
 </file>
@@ -585,7 +591,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -643,7 +649,6 @@
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="32" applyFont="1"/>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="31" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -691,6 +696,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>474705</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>44451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A770E37F-B482-C48F-69E5-AB265CCAA341}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="1841501"/>
+          <a:ext cx="6532605" cy="4648200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -983,7 +1037,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1022,6 +1076,16 @@
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
     </row>
@@ -1040,6 +1104,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6593,7 +6658,7 @@
   <dimension ref="A1:AF59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D4" sqref="D4:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6609,7 +6674,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
+      <c r="A2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -6716,44 +6781,44 @@
         <v>1697.08</v>
       </c>
       <c r="D4">
-        <f>D9*0.25</f>
-        <v>1020.0425</v>
+        <f>D9*(1-0.56)</f>
+        <v>1795.2747999999999</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:M4" si="0">E9*0.25</f>
-        <v>1000.8575</v>
+        <f t="shared" ref="E4:M4" si="0">E9*(1-0.56)</f>
+        <v>1761.5091999999997</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>1102.7774999999999</v>
+        <v>1940.8883999999996</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1057.2825</v>
+        <v>1860.8171999999997</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>1022.79</v>
+        <v>1800.1103999999998</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>1024.8150000000001</v>
+        <v>1803.6743999999999</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>1031.5474999999999</v>
+        <v>1815.5235999999995</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>1089.8074999999999</v>
+        <v>1918.0611999999996</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>1145.5925</v>
+        <v>2016.2427999999998</v>
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>1156.375</v>
+        <v>2035.2199999999998</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -6821,44 +6886,44 @@
         <v>3617.05</v>
       </c>
       <c r="D5">
-        <f>D10*0.25</f>
-        <v>1020.0425</v>
+        <f>D10*(1-0.56)</f>
+        <v>1795.2747999999999</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:M5" si="1">E10*0.25</f>
-        <v>1000.8575</v>
+        <f t="shared" ref="E5:M5" si="1">E10*(1-0.56)</f>
+        <v>1761.5091999999997</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>1102.7774999999999</v>
+        <v>1940.8883999999996</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>1057.2825</v>
+        <v>1860.8171999999997</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>1022.79</v>
+        <v>1800.1103999999998</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>1024.8150000000001</v>
+        <v>1803.6743999999999</v>
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
-        <v>1031.5474999999999</v>
+        <v>1815.5235999999995</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>1089.8074999999999</v>
+        <v>1918.0611999999996</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>1145.5925</v>
+        <v>2016.2427999999998</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>1156.375</v>
+        <v>2035.2199999999998</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -8131,43 +8196,43 @@
       </c>
       <c r="E46" s="5">
         <f t="shared" si="5"/>
-        <v>1596.4939681335359</v>
+        <v>2371.7262681335355</v>
       </c>
       <c r="F46" s="5">
         <f t="shared" si="5"/>
-        <v>1569.1826100151745</v>
+        <v>2329.8343100151742</v>
       </c>
       <c r="G46" s="5">
         <f t="shared" si="5"/>
-        <v>1671.1026100151744</v>
+        <v>2509.2135100151741</v>
       </c>
       <c r="H46" s="5">
         <f t="shared" si="5"/>
-        <v>1625.6076100151745</v>
+        <v>2429.1423100151742</v>
       </c>
       <c r="I46" s="5">
         <f t="shared" si="5"/>
-        <v>1591.1151100151747</v>
+        <v>2368.4355100151743</v>
       </c>
       <c r="J46" s="5">
         <f t="shared" si="5"/>
-        <v>1593.1401100151747</v>
+        <v>2371.9995100151746</v>
       </c>
       <c r="K46" s="5">
         <f t="shared" si="5"/>
-        <v>1599.8726100151744</v>
+        <v>2383.8487100151742</v>
       </c>
       <c r="L46" s="5">
         <f t="shared" si="5"/>
-        <v>1658.1326100151746</v>
+        <v>2486.3863100151743</v>
       </c>
       <c r="M46" s="5">
         <f t="shared" si="5"/>
-        <v>1713.9176100151744</v>
+        <v>2584.5679100151742</v>
       </c>
       <c r="N46" s="5">
         <f t="shared" si="5"/>
-        <v>1724.7001100151747</v>
+        <v>2603.5451100151745</v>
       </c>
       <c r="O46" s="5">
         <f t="shared" si="5"/>
@@ -8256,43 +8321,43 @@
       </c>
       <c r="E47" s="5">
         <f t="shared" si="6"/>
-        <v>1596.4939681335359</v>
+        <v>2371.7262681335355</v>
       </c>
       <c r="F47" s="5">
         <f t="shared" si="6"/>
-        <v>1569.1826100151745</v>
+        <v>2329.8343100151742</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" si="6"/>
-        <v>1671.1026100151744</v>
+        <v>2509.2135100151741</v>
       </c>
       <c r="H47" s="5">
         <f t="shared" si="6"/>
-        <v>1625.6076100151745</v>
+        <v>2429.1423100151742</v>
       </c>
       <c r="I47" s="5">
         <f t="shared" si="6"/>
-        <v>1591.1151100151747</v>
+        <v>2368.4355100151743</v>
       </c>
       <c r="J47" s="5">
         <f t="shared" si="6"/>
-        <v>1593.1401100151747</v>
+        <v>2371.9995100151746</v>
       </c>
       <c r="K47" s="5">
         <f t="shared" si="6"/>
-        <v>1599.8726100151744</v>
+        <v>2383.8487100151742</v>
       </c>
       <c r="L47" s="5">
         <f t="shared" si="6"/>
-        <v>1658.1326100151746</v>
+        <v>2486.3863100151743</v>
       </c>
       <c r="M47" s="5">
         <f t="shared" si="6"/>
-        <v>1713.9176100151744</v>
+        <v>2584.5679100151742</v>
       </c>
       <c r="N47" s="5">
         <f t="shared" si="6"/>
-        <v>1724.7001100151747</v>
+        <v>2603.5451100151745</v>
       </c>
       <c r="O47" s="5">
         <f t="shared" si="6"/>
@@ -10395,43 +10460,43 @@
       </c>
       <c r="D2" s="19">
         <f>'Passenger Vehicle Calculations'!E46</f>
-        <v>1596.4939681335359</v>
+        <v>2371.7262681335355</v>
       </c>
       <c r="E2" s="19">
         <f>'Passenger Vehicle Calculations'!F46</f>
-        <v>1569.1826100151745</v>
+        <v>2329.8343100151742</v>
       </c>
       <c r="F2" s="19">
         <f>'Passenger Vehicle Calculations'!G46</f>
-        <v>1671.1026100151744</v>
+        <v>2509.2135100151741</v>
       </c>
       <c r="G2" s="19">
         <f>'Passenger Vehicle Calculations'!H46</f>
-        <v>1625.6076100151745</v>
+        <v>2429.1423100151742</v>
       </c>
       <c r="H2" s="19">
         <f>'Passenger Vehicle Calculations'!I46</f>
-        <v>1591.1151100151747</v>
+        <v>2368.4355100151743</v>
       </c>
       <c r="I2" s="19">
         <f>'Passenger Vehicle Calculations'!J46</f>
-        <v>1593.1401100151747</v>
+        <v>2371.9995100151746</v>
       </c>
       <c r="J2" s="19">
         <f>'Passenger Vehicle Calculations'!K46</f>
-        <v>1599.8726100151744</v>
+        <v>2383.8487100151742</v>
       </c>
       <c r="K2" s="19">
         <f>'Passenger Vehicle Calculations'!L46</f>
-        <v>1658.1326100151746</v>
+        <v>2486.3863100151743</v>
       </c>
       <c r="L2" s="19">
         <f>'Passenger Vehicle Calculations'!M46</f>
-        <v>1713.9176100151744</v>
+        <v>2584.5679100151742</v>
       </c>
       <c r="M2" s="19">
         <f>'Passenger Vehicle Calculations'!N46</f>
-        <v>1724.7001100151747</v>
+        <v>2603.5451100151745</v>
       </c>
       <c r="N2" s="19">
         <f>'Passenger Vehicle Calculations'!O46</f>
@@ -10805,43 +10870,43 @@
       </c>
       <c r="D6" s="19">
         <f>'Passenger Vehicle Calculations'!E47</f>
-        <v>1596.4939681335359</v>
+        <v>2371.7262681335355</v>
       </c>
       <c r="E6" s="19">
         <f>'Passenger Vehicle Calculations'!F47</f>
-        <v>1569.1826100151745</v>
+        <v>2329.8343100151742</v>
       </c>
       <c r="F6" s="19">
         <f>'Passenger Vehicle Calculations'!G47</f>
-        <v>1671.1026100151744</v>
+        <v>2509.2135100151741</v>
       </c>
       <c r="G6" s="19">
         <f>'Passenger Vehicle Calculations'!H47</f>
-        <v>1625.6076100151745</v>
+        <v>2429.1423100151742</v>
       </c>
       <c r="H6" s="19">
         <f>'Passenger Vehicle Calculations'!I47</f>
-        <v>1591.1151100151747</v>
+        <v>2368.4355100151743</v>
       </c>
       <c r="I6" s="19">
         <f>'Passenger Vehicle Calculations'!J47</f>
-        <v>1593.1401100151747</v>
+        <v>2371.9995100151746</v>
       </c>
       <c r="J6" s="19">
         <f>'Passenger Vehicle Calculations'!K47</f>
-        <v>1599.8726100151744</v>
+        <v>2383.8487100151742</v>
       </c>
       <c r="K6" s="19">
         <f>'Passenger Vehicle Calculations'!L47</f>
-        <v>1658.1326100151746</v>
+        <v>2486.3863100151743</v>
       </c>
       <c r="L6" s="19">
         <f>'Passenger Vehicle Calculations'!M47</f>
-        <v>1713.9176100151744</v>
+        <v>2584.5679100151742</v>
       </c>
       <c r="M6" s="19">
         <f>'Passenger Vehicle Calculations'!N47</f>
-        <v>1724.7001100151747</v>
+        <v>2603.5451100151745</v>
       </c>
       <c r="N6" s="19">
         <f>'Passenger Vehicle Calculations'!O47</f>
@@ -11023,43 +11088,43 @@
       </c>
       <c r="D8" s="19">
         <f>D2</f>
-        <v>1596.4939681335359</v>
+        <v>2371.7262681335355</v>
       </c>
       <c r="E8" s="19">
         <f t="shared" ref="E8:AE8" si="0">E2</f>
-        <v>1569.1826100151745</v>
+        <v>2329.8343100151742</v>
       </c>
       <c r="F8" s="19">
         <f t="shared" si="0"/>
-        <v>1671.1026100151744</v>
+        <v>2509.2135100151741</v>
       </c>
       <c r="G8" s="19">
         <f t="shared" si="0"/>
-        <v>1625.6076100151745</v>
+        <v>2429.1423100151742</v>
       </c>
       <c r="H8" s="19">
         <f t="shared" si="0"/>
-        <v>1591.1151100151747</v>
+        <v>2368.4355100151743</v>
       </c>
       <c r="I8" s="19">
         <f t="shared" si="0"/>
-        <v>1593.1401100151747</v>
+        <v>2371.9995100151746</v>
       </c>
       <c r="J8" s="19">
         <f t="shared" si="0"/>
-        <v>1599.8726100151744</v>
+        <v>2383.8487100151742</v>
       </c>
       <c r="K8" s="19">
         <f t="shared" si="0"/>
-        <v>1658.1326100151746</v>
+        <v>2486.3863100151743</v>
       </c>
       <c r="L8" s="19">
         <f t="shared" si="0"/>
-        <v>1713.9176100151744</v>
+        <v>2584.5679100151742</v>
       </c>
       <c r="M8" s="19">
         <f t="shared" si="0"/>
-        <v>1724.7001100151747</v>
+        <v>2603.5451100151745</v>
       </c>
       <c r="N8" s="19">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Edit to FEOC values for vehicle subsidies after 2025
</commit_message>
<xml_diff>
--- a/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
+++ b/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDA6C5A-A488-4546-90F0-F5782A95BD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B291C5C-0D68-4026-BF5B-12E51E7484B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="730" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -303,13 +303,13 @@
     <t>values from original IRA analysis</t>
   </si>
   <si>
-    <t>values assuming a 56% cut in our original analysis to represent FEOC restrictions</t>
-  </si>
-  <si>
     <t>Foreign Entities of Concern Multiplier</t>
   </si>
   <si>
     <t>BloombergNEF, MarkLines, Department of Energy</t>
+  </si>
+  <si>
+    <t>We assume a 56% cut in our original analysis to represent FEOC restrictions for the year 2024, based on BNEF data. We assume more restrictive guidance starting in 2025 will reduce the credit amount by 75%.</t>
   </si>
 </sst>
 </file>
@@ -1078,12 +1078,12 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -6657,8 +6657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A3CC6-8591-4A07-9E4B-1DE39D29E87F}">
   <dimension ref="A1:AF59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:M5"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6675,7 +6675,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
@@ -6789,36 +6789,36 @@
         <v>1761.5091999999997</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
-        <v>1940.8883999999996</v>
+        <f>F9*(1-0.75)</f>
+        <v>1102.7774999999999</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>1860.8171999999997</v>
+        <f t="shared" ref="G4:M4" si="1">G9*(1-0.75)</f>
+        <v>1057.2825</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
-        <v>1800.1103999999998</v>
+        <f t="shared" si="1"/>
+        <v>1022.79</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>1803.6743999999999</v>
+        <f t="shared" si="1"/>
+        <v>1024.8150000000001</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
-        <v>1815.5235999999995</v>
+        <f t="shared" si="1"/>
+        <v>1031.5474999999999</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
-        <v>1918.0611999999996</v>
+        <f t="shared" si="1"/>
+        <v>1089.8074999999999</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
-        <v>2016.2427999999998</v>
+        <f t="shared" si="1"/>
+        <v>1145.5925</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
-        <v>2035.2199999999998</v>
+        <f t="shared" si="1"/>
+        <v>1156.375</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -6890,40 +6890,40 @@
         <v>1795.2747999999999</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:M5" si="1">E10*(1-0.56)</f>
+        <f t="shared" ref="E5:M5" si="2">E10*(1-0.56)</f>
         <v>1761.5091999999997</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
-        <v>1940.8883999999996</v>
+        <f>F10*(1-0.75)</f>
+        <v>1102.7774999999999</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
-        <v>1860.8171999999997</v>
+        <f t="shared" ref="G5:M5" si="3">G10*(1-0.75)</f>
+        <v>1057.2825</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>1800.1103999999998</v>
+        <f t="shared" si="3"/>
+        <v>1022.79</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
-        <v>1803.6743999999999</v>
+        <f t="shared" si="3"/>
+        <v>1024.8150000000001</v>
       </c>
       <c r="J5">
-        <f t="shared" si="1"/>
-        <v>1815.5235999999995</v>
+        <f t="shared" si="3"/>
+        <v>1031.5474999999999</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
-        <v>1918.0611999999996</v>
+        <f t="shared" si="3"/>
+        <v>1089.8074999999999</v>
       </c>
       <c r="L5">
-        <f t="shared" si="1"/>
-        <v>2016.2427999999998</v>
+        <f t="shared" si="3"/>
+        <v>1145.5925</v>
       </c>
       <c r="M5">
-        <f t="shared" si="1"/>
-        <v>2035.2199999999998</v>
+        <f t="shared" si="3"/>
+        <v>1156.375</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -7332,27 +7332,27 @@
         <v>2020</v>
       </c>
       <c r="E19" s="8">
-        <f t="shared" ref="E19:J19" si="2">D19+1</f>
+        <f t="shared" ref="E19:J19" si="4">D19+1</f>
         <v>2021</v>
       </c>
       <c r="F19" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2022</v>
       </c>
       <c r="G19" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2023</v>
       </c>
       <c r="H19" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2024</v>
       </c>
       <c r="I19" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2025</v>
       </c>
       <c r="J19" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2026</v>
       </c>
     </row>
@@ -7961,27 +7961,27 @@
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.35">
       <c r="C42" s="5">
-        <f t="shared" ref="C42:H42" si="3">SUMPRODUCT(E20:E33,$B$20:$B$33)/SUM($B$20:$B$33)*$B$38</f>
+        <f t="shared" ref="C42:H42" si="5">SUMPRODUCT(E20:E33,$B$20:$B$33)/SUM($B$20:$B$33)*$B$38</f>
         <v>600.15334597875574</v>
       </c>
       <c r="D42" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>576.45146813353574</v>
       </c>
       <c r="E42" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>576.45146813353574</v>
       </c>
       <c r="F42" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>568.32511001517457</v>
       </c>
       <c r="G42" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>568.32511001517457</v>
       </c>
       <c r="H42" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>568.32511001517457</v>
       </c>
       <c r="I42" s="5">
@@ -7989,95 +7989,95 @@
         <v>568.32511001517457</v>
       </c>
       <c r="J42" s="5">
-        <f t="shared" ref="J42:AF42" si="4">I42</f>
+        <f t="shared" ref="J42:AF42" si="6">I42</f>
         <v>568.32511001517457</v>
       </c>
       <c r="K42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="L42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="M42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="N42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="O42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="P42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="Q42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="R42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="S42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="T42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="U42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="V42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="W42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="X42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="Y42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="Z42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AA42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AB42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AC42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AD42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AE42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AF42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>568.32511001517457</v>
       </c>
     </row>
@@ -8187,123 +8187,123 @@
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5">
-        <f t="shared" ref="C46:AF46" si="5">B4+C42</f>
+        <f t="shared" ref="C46:AF46" si="7">B4+C42</f>
         <v>3036.0333459787557</v>
       </c>
       <c r="D46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2273.5314681335358</v>
       </c>
       <c r="E46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2371.7262681335355</v>
       </c>
       <c r="F46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2329.8343100151742</v>
       </c>
       <c r="G46" s="5">
-        <f t="shared" si="5"/>
-        <v>2509.2135100151741</v>
+        <f t="shared" si="7"/>
+        <v>1671.1026100151744</v>
       </c>
       <c r="H46" s="5">
-        <f t="shared" si="5"/>
-        <v>2429.1423100151742</v>
+        <f t="shared" si="7"/>
+        <v>1625.6076100151745</v>
       </c>
       <c r="I46" s="5">
-        <f t="shared" si="5"/>
-        <v>2368.4355100151743</v>
+        <f t="shared" si="7"/>
+        <v>1591.1151100151747</v>
       </c>
       <c r="J46" s="5">
-        <f t="shared" si="5"/>
-        <v>2371.9995100151746</v>
+        <f t="shared" si="7"/>
+        <v>1593.1401100151747</v>
       </c>
       <c r="K46" s="5">
-        <f t="shared" si="5"/>
-        <v>2383.8487100151742</v>
+        <f t="shared" si="7"/>
+        <v>1599.8726100151744</v>
       </c>
       <c r="L46" s="5">
-        <f t="shared" si="5"/>
-        <v>2486.3863100151743</v>
+        <f t="shared" si="7"/>
+        <v>1658.1326100151746</v>
       </c>
       <c r="M46" s="5">
-        <f t="shared" si="5"/>
-        <v>2584.5679100151742</v>
+        <f t="shared" si="7"/>
+        <v>1713.9176100151744</v>
       </c>
       <c r="N46" s="5">
-        <f t="shared" si="5"/>
-        <v>2603.5451100151745</v>
+        <f t="shared" si="7"/>
+        <v>1724.7001100151747</v>
       </c>
       <c r="O46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="P46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="Q46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="R46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="S46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="T46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="U46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="V46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="W46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="X46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="Y46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="Z46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AA46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AB46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AC46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AD46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AE46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AF46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>568.32511001517457</v>
       </c>
     </row>
@@ -8312,123 +8312,123 @@
         <v>46</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" ref="C47:AF47" si="6">B5+C42</f>
+        <f t="shared" ref="C47:AF47" si="8">B5+C42</f>
         <v>7252.8733459787563</v>
       </c>
       <c r="D47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4193.501468133536</v>
       </c>
       <c r="E47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2371.7262681335355</v>
       </c>
       <c r="F47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2329.8343100151742</v>
       </c>
       <c r="G47" s="5">
-        <f t="shared" si="6"/>
-        <v>2509.2135100151741</v>
+        <f t="shared" si="8"/>
+        <v>1671.1026100151744</v>
       </c>
       <c r="H47" s="5">
-        <f t="shared" si="6"/>
-        <v>2429.1423100151742</v>
+        <f t="shared" si="8"/>
+        <v>1625.6076100151745</v>
       </c>
       <c r="I47" s="5">
-        <f t="shared" si="6"/>
-        <v>2368.4355100151743</v>
+        <f t="shared" si="8"/>
+        <v>1591.1151100151747</v>
       </c>
       <c r="J47" s="5">
-        <f t="shared" si="6"/>
-        <v>2371.9995100151746</v>
+        <f t="shared" si="8"/>
+        <v>1593.1401100151747</v>
       </c>
       <c r="K47" s="5">
-        <f t="shared" si="6"/>
-        <v>2383.8487100151742</v>
+        <f t="shared" si="8"/>
+        <v>1599.8726100151744</v>
       </c>
       <c r="L47" s="5">
-        <f t="shared" si="6"/>
-        <v>2486.3863100151743</v>
+        <f t="shared" si="8"/>
+        <v>1658.1326100151746</v>
       </c>
       <c r="M47" s="5">
-        <f t="shared" si="6"/>
-        <v>2584.5679100151742</v>
+        <f t="shared" si="8"/>
+        <v>1713.9176100151744</v>
       </c>
       <c r="N47" s="5">
-        <f t="shared" si="6"/>
-        <v>2603.5451100151745</v>
+        <f t="shared" si="8"/>
+        <v>1724.7001100151747</v>
       </c>
       <c r="O47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="P47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="Q47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="R47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="S47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="T47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="U47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="V47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="W47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="X47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="Y47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="Z47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AA47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AB47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AC47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AD47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AE47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
       <c r="AF47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>568.32511001517457</v>
       </c>
     </row>
@@ -10468,35 +10468,35 @@
       </c>
       <c r="F2" s="19">
         <f>'Passenger Vehicle Calculations'!G46</f>
-        <v>2509.2135100151741</v>
+        <v>1671.1026100151744</v>
       </c>
       <c r="G2" s="19">
         <f>'Passenger Vehicle Calculations'!H46</f>
-        <v>2429.1423100151742</v>
+        <v>1625.6076100151745</v>
       </c>
       <c r="H2" s="19">
         <f>'Passenger Vehicle Calculations'!I46</f>
-        <v>2368.4355100151743</v>
+        <v>1591.1151100151747</v>
       </c>
       <c r="I2" s="19">
         <f>'Passenger Vehicle Calculations'!J46</f>
-        <v>2371.9995100151746</v>
+        <v>1593.1401100151747</v>
       </c>
       <c r="J2" s="19">
         <f>'Passenger Vehicle Calculations'!K46</f>
-        <v>2383.8487100151742</v>
+        <v>1599.8726100151744</v>
       </c>
       <c r="K2" s="19">
         <f>'Passenger Vehicle Calculations'!L46</f>
-        <v>2486.3863100151743</v>
+        <v>1658.1326100151746</v>
       </c>
       <c r="L2" s="19">
         <f>'Passenger Vehicle Calculations'!M46</f>
-        <v>2584.5679100151742</v>
+        <v>1713.9176100151744</v>
       </c>
       <c r="M2" s="19">
         <f>'Passenger Vehicle Calculations'!N46</f>
-        <v>2603.5451100151745</v>
+        <v>1724.7001100151747</v>
       </c>
       <c r="N2" s="19">
         <f>'Passenger Vehicle Calculations'!O46</f>
@@ -10878,35 +10878,35 @@
       </c>
       <c r="F6" s="19">
         <f>'Passenger Vehicle Calculations'!G47</f>
-        <v>2509.2135100151741</v>
+        <v>1671.1026100151744</v>
       </c>
       <c r="G6" s="19">
         <f>'Passenger Vehicle Calculations'!H47</f>
-        <v>2429.1423100151742</v>
+        <v>1625.6076100151745</v>
       </c>
       <c r="H6" s="19">
         <f>'Passenger Vehicle Calculations'!I47</f>
-        <v>2368.4355100151743</v>
+        <v>1591.1151100151747</v>
       </c>
       <c r="I6" s="19">
         <f>'Passenger Vehicle Calculations'!J47</f>
-        <v>2371.9995100151746</v>
+        <v>1593.1401100151747</v>
       </c>
       <c r="J6" s="19">
         <f>'Passenger Vehicle Calculations'!K47</f>
-        <v>2383.8487100151742</v>
+        <v>1599.8726100151744</v>
       </c>
       <c r="K6" s="19">
         <f>'Passenger Vehicle Calculations'!L47</f>
-        <v>2486.3863100151743</v>
+        <v>1658.1326100151746</v>
       </c>
       <c r="L6" s="19">
         <f>'Passenger Vehicle Calculations'!M47</f>
-        <v>2584.5679100151742</v>
+        <v>1713.9176100151744</v>
       </c>
       <c r="M6" s="19">
         <f>'Passenger Vehicle Calculations'!N47</f>
-        <v>2603.5451100151745</v>
+        <v>1724.7001100151747</v>
       </c>
       <c r="N6" s="19">
         <f>'Passenger Vehicle Calculations'!O47</f>
@@ -11096,35 +11096,35 @@
       </c>
       <c r="F8" s="19">
         <f t="shared" si="0"/>
-        <v>2509.2135100151741</v>
+        <v>1671.1026100151744</v>
       </c>
       <c r="G8" s="19">
         <f t="shared" si="0"/>
-        <v>2429.1423100151742</v>
+        <v>1625.6076100151745</v>
       </c>
       <c r="H8" s="19">
         <f t="shared" si="0"/>
-        <v>2368.4355100151743</v>
+        <v>1591.1151100151747</v>
       </c>
       <c r="I8" s="19">
         <f t="shared" si="0"/>
-        <v>2371.9995100151746</v>
+        <v>1593.1401100151747</v>
       </c>
       <c r="J8" s="19">
         <f t="shared" si="0"/>
-        <v>2383.8487100151742</v>
+        <v>1599.8726100151744</v>
       </c>
       <c r="K8" s="19">
         <f t="shared" si="0"/>
-        <v>2486.3863100151743</v>
+        <v>1658.1326100151746</v>
       </c>
       <c r="L8" s="19">
         <f t="shared" si="0"/>
-        <v>2584.5679100151742</v>
+        <v>1713.9176100151744</v>
       </c>
       <c r="M8" s="19">
         <f t="shared" si="0"/>
-        <v>2603.5451100151745</v>
+        <v>1724.7001100151747</v>
       </c>
       <c r="N8" s="19">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Update state PHEV subsidies
</commit_message>
<xml_diff>
--- a/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
+++ b/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\trans\BVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB5F82D-4199-462E-956F-98B9574200DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116D7EF2-3C86-4E89-8090-35539B011F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58740" yWindow="1140" windowWidth="23910" windowHeight="14415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35745" yWindow="1065" windowWidth="21660" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -6949,8 +6949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A3CC6-8591-4A07-9E4B-1DE39D29E87F}">
   <dimension ref="A1:AG109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O52" sqref="O52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8616,19 +8616,19 @@
         <v>21</v>
       </c>
       <c r="D47" s="8">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E47" s="8">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="F47" s="8">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G47" s="8">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H47" s="8">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I47" s="8">
         <v>0</v>
@@ -8721,16 +8721,17 @@
         <v>2500</v>
       </c>
       <c r="G50" s="8">
-        <v>3500</v>
+        <f>G30*0.5</f>
+        <v>1750</v>
       </c>
       <c r="H50" s="8">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="I50" s="8">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="J50" s="8">
-        <v>3500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8754,16 +8755,16 @@
         <v>0</v>
       </c>
       <c r="G51" s="8">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="H51" s="8">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="I51" s="8">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="J51" s="8">
-        <v>3000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="52" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8783,19 +8784,19 @@
         <v>0</v>
       </c>
       <c r="F52" s="8">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="G52" s="8">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="H52" s="8">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="I52" s="8">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="J52" s="8">
-        <v>1500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="53" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8818,16 +8819,16 @@
         <v>2000</v>
       </c>
       <c r="G53" s="8">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="H53" s="8">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="I53" s="8">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="J53" s="8">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8880,25 +8881,25 @@
         <v>21</v>
       </c>
       <c r="D55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="E55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="F55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="G55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="H55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="I55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="J55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="56" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -9199,127 +9200,127 @@
       </c>
       <c r="C66" s="5">
         <f>SUMPRODUCT(D40:D56,$B$40:$B$56)/SUM($B$40:$B$56)*K$79</f>
-        <v>463.29350546214374</v>
+        <v>457.66715073896358</v>
       </c>
       <c r="D66" s="5">
         <f t="shared" ref="D66:I66" si="16">SUMPRODUCT(E40:E56,$B$40:$B$56)/SUM($B$40:$B$56)*L$79</f>
-        <v>221.09557242733794</v>
+        <v>215.72168420258612</v>
       </c>
       <c r="E66" s="5">
         <f t="shared" si="16"/>
-        <v>194.30618610622579</v>
+        <v>188.02811316670545</v>
       </c>
       <c r="F66" s="5">
         <f t="shared" si="16"/>
-        <v>255.3303083708262</v>
+        <v>181.15698643889937</v>
       </c>
       <c r="G66" s="5">
         <f t="shared" si="16"/>
-        <v>251.52892263302851</v>
+        <v>152.76346597230366</v>
       </c>
       <c r="H66" s="5">
         <f t="shared" si="16"/>
-        <v>189.20535092319807</v>
+        <v>96.20855199074947</v>
       </c>
       <c r="I66" s="5">
         <f t="shared" si="16"/>
-        <v>183.69451545941558</v>
+        <v>93.406361156067433</v>
       </c>
       <c r="J66" s="5">
         <f t="shared" ref="J66:R66" si="17">I66*R$79/Q$79</f>
-        <v>178.34418976642291</v>
+        <v>90.685787530162571</v>
       </c>
       <c r="K66" s="5">
         <f t="shared" si="17"/>
-        <v>173.14969880235233</v>
+        <v>88.04445391277919</v>
       </c>
       <c r="L66" s="5">
         <f t="shared" si="17"/>
-        <v>168.10650369160422</v>
+        <v>85.480052342504052</v>
       </c>
       <c r="M66" s="5">
         <f t="shared" si="17"/>
-        <v>163.21019775883906</v>
+        <v>82.990342080101016</v>
       </c>
       <c r="N66" s="5">
         <f t="shared" si="17"/>
-        <v>158.45650267848453</v>
+        <v>80.573147650583522</v>
       </c>
       <c r="O66" s="5">
         <f t="shared" si="17"/>
-        <v>153.8412647363927</v>
+        <v>78.226356942314084</v>
       </c>
       <c r="P66" s="5">
         <f t="shared" si="17"/>
-        <v>149.36045120038131</v>
+        <v>75.947919361469985</v>
       </c>
       <c r="Q66" s="5">
         <f t="shared" si="17"/>
-        <v>145.01014679648668</v>
+        <v>73.735844040262123</v>
       </c>
       <c r="R66" s="5">
         <f t="shared" si="17"/>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="S66" s="5">
         <f t="shared" ref="S66" si="18">R66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="T66" s="5">
         <f t="shared" ref="T66" si="19">S66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="U66" s="5">
         <f t="shared" ref="U66" si="20">T66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="V66" s="5">
         <f t="shared" ref="V66" si="21">U66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="W66" s="5">
         <f t="shared" ref="W66" si="22">V66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="X66" s="5">
         <f t="shared" ref="X66" si="23">W66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="Y66" s="5">
         <f t="shared" ref="Y66" si="24">X66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="Z66" s="5">
         <f t="shared" ref="Z66" si="25">Y66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AA66" s="5">
         <f t="shared" ref="AA66" si="26">Z66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AB66" s="5">
         <f t="shared" ref="AB66" si="27">AA66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AC66" s="5">
         <f t="shared" ref="AC66" si="28">AB66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AD66" s="5">
         <f t="shared" ref="AD66" si="29">AC66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AE66" s="5">
         <f t="shared" ref="AE66" si="30">AD66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AF66" s="5">
         <f t="shared" ref="AF66" si="31">AE66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AG66" s="5">
         <f t="shared" ref="AG66" si="32">AF66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Revert "Update state PHEV subsidies"
This reverts commit 1454aed352df3df62fa041fed4290abaf61841b1.
</commit_message>
<xml_diff>
--- a/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
+++ b/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\trans\BVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116D7EF2-3C86-4E89-8090-35539B011F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB5F82D-4199-462E-956F-98B9574200DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35745" yWindow="1065" windowWidth="21660" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58740" yWindow="1140" windowWidth="23910" windowHeight="14415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -6949,8 +6949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A3CC6-8591-4A07-9E4B-1DE39D29E87F}">
   <dimension ref="A1:AG109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R53" sqref="R53"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8616,19 +8616,19 @@
         <v>21</v>
       </c>
       <c r="D47" s="8">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E47" s="8">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F47" s="8">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G47" s="8">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="H47" s="8">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I47" s="8">
         <v>0</v>
@@ -8721,17 +8721,16 @@
         <v>2500</v>
       </c>
       <c r="G50" s="8">
-        <f>G30*0.5</f>
-        <v>1750</v>
+        <v>3500</v>
       </c>
       <c r="H50" s="8">
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="I50" s="8">
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="J50" s="8">
-        <v>0</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="51" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8755,16 +8754,16 @@
         <v>0</v>
       </c>
       <c r="G51" s="8">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="H51" s="8">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="I51" s="8">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="J51" s="8">
-        <v>1500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="52" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8784,19 +8783,19 @@
         <v>0</v>
       </c>
       <c r="F52" s="8">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="G52" s="8">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="H52" s="8">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="I52" s="8">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J52" s="8">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="53" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8819,16 +8818,16 @@
         <v>2000</v>
       </c>
       <c r="G53" s="8">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="H53" s="8">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="I53" s="8">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="J53" s="8">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="54" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8881,25 +8880,25 @@
         <v>21</v>
       </c>
       <c r="D55" s="43">
-        <v>1000</v>
+        <v>2200</v>
       </c>
       <c r="E55" s="43">
-        <v>1000</v>
+        <v>2200</v>
       </c>
       <c r="F55" s="43">
-        <v>1000</v>
+        <v>2200</v>
       </c>
       <c r="G55" s="43">
-        <v>1000</v>
+        <v>2200</v>
       </c>
       <c r="H55" s="43">
-        <v>1000</v>
+        <v>2200</v>
       </c>
       <c r="I55" s="43">
-        <v>1000</v>
+        <v>2200</v>
       </c>
       <c r="J55" s="43">
-        <v>1000</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="56" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -9200,127 +9199,127 @@
       </c>
       <c r="C66" s="5">
         <f>SUMPRODUCT(D40:D56,$B$40:$B$56)/SUM($B$40:$B$56)*K$79</f>
-        <v>457.66715073896358</v>
+        <v>463.29350546214374</v>
       </c>
       <c r="D66" s="5">
         <f t="shared" ref="D66:I66" si="16">SUMPRODUCT(E40:E56,$B$40:$B$56)/SUM($B$40:$B$56)*L$79</f>
-        <v>215.72168420258612</v>
+        <v>221.09557242733794</v>
       </c>
       <c r="E66" s="5">
         <f t="shared" si="16"/>
-        <v>188.02811316670545</v>
+        <v>194.30618610622579</v>
       </c>
       <c r="F66" s="5">
         <f t="shared" si="16"/>
-        <v>181.15698643889937</v>
+        <v>255.3303083708262</v>
       </c>
       <c r="G66" s="5">
         <f t="shared" si="16"/>
-        <v>152.76346597230366</v>
+        <v>251.52892263302851</v>
       </c>
       <c r="H66" s="5">
         <f t="shared" si="16"/>
-        <v>96.20855199074947</v>
+        <v>189.20535092319807</v>
       </c>
       <c r="I66" s="5">
         <f t="shared" si="16"/>
-        <v>93.406361156067433</v>
+        <v>183.69451545941558</v>
       </c>
       <c r="J66" s="5">
         <f t="shared" ref="J66:R66" si="17">I66*R$79/Q$79</f>
-        <v>90.685787530162571</v>
+        <v>178.34418976642291</v>
       </c>
       <c r="K66" s="5">
         <f t="shared" si="17"/>
-        <v>88.04445391277919</v>
+        <v>173.14969880235233</v>
       </c>
       <c r="L66" s="5">
         <f t="shared" si="17"/>
-        <v>85.480052342504052</v>
+        <v>168.10650369160422</v>
       </c>
       <c r="M66" s="5">
         <f t="shared" si="17"/>
-        <v>82.990342080101016</v>
+        <v>163.21019775883906</v>
       </c>
       <c r="N66" s="5">
         <f t="shared" si="17"/>
-        <v>80.573147650583522</v>
+        <v>158.45650267848453</v>
       </c>
       <c r="O66" s="5">
         <f t="shared" si="17"/>
-        <v>78.226356942314084</v>
+        <v>153.8412647363927</v>
       </c>
       <c r="P66" s="5">
         <f t="shared" si="17"/>
-        <v>75.947919361469985</v>
+        <v>149.36045120038131</v>
       </c>
       <c r="Q66" s="5">
         <f t="shared" si="17"/>
-        <v>73.735844040262123</v>
+        <v>145.01014679648668</v>
       </c>
       <c r="R66" s="5">
         <f t="shared" si="17"/>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="S66" s="5">
         <f t="shared" ref="S66" si="18">R66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="T66" s="5">
         <f t="shared" ref="T66" si="19">S66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="U66" s="5">
         <f t="shared" ref="U66" si="20">T66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="V66" s="5">
         <f t="shared" ref="V66" si="21">U66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="W66" s="5">
         <f t="shared" ref="W66" si="22">V66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="X66" s="5">
         <f t="shared" ref="X66" si="23">W66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="Y66" s="5">
         <f t="shared" ref="Y66" si="24">X66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="Z66" s="5">
         <f t="shared" ref="Z66" si="25">Y66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="AA66" s="5">
         <f t="shared" ref="AA66" si="26">Z66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="AB66" s="5">
         <f t="shared" ref="AB66" si="27">AA66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="AC66" s="5">
         <f t="shared" ref="AC66" si="28">AB66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="AD66" s="5">
         <f t="shared" ref="AD66" si="29">AC66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="AE66" s="5">
         <f t="shared" ref="AE66" si="30">AD66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="AF66" s="5">
         <f t="shared" ref="AF66" si="31">AE66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
       <c r="AG66" s="5">
         <f t="shared" ref="AG66" si="32">AF66</f>
-        <v>71.588198097341873</v>
+        <v>140.78655028785116</v>
       </c>
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update state PHEV subsidies (formula fix)
</commit_message>
<xml_diff>
--- a/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
+++ b/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\trans\BVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB5F82D-4199-462E-956F-98B9574200DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198C8C8B-8C14-4E6F-8DC9-713862856D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58740" yWindow="1140" windowWidth="23910" windowHeight="14415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60630" yWindow="2445" windowWidth="23910" windowHeight="14415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -6949,8 +6949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A3CC6-8591-4A07-9E4B-1DE39D29E87F}">
   <dimension ref="A1:AG109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O52" sqref="O52"/>
+    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8616,19 +8616,19 @@
         <v>21</v>
       </c>
       <c r="D47" s="8">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E47" s="8">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="F47" s="8">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G47" s="8">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H47" s="8">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I47" s="8">
         <v>0</v>
@@ -8721,16 +8721,17 @@
         <v>2500</v>
       </c>
       <c r="G50" s="8">
-        <v>3500</v>
+        <f>G30*0.5</f>
+        <v>1750</v>
       </c>
       <c r="H50" s="8">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="I50" s="8">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="J50" s="8">
-        <v>3500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8754,16 +8755,16 @@
         <v>0</v>
       </c>
       <c r="G51" s="8">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="H51" s="8">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="I51" s="8">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="J51" s="8">
-        <v>3000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="52" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8783,19 +8784,19 @@
         <v>0</v>
       </c>
       <c r="F52" s="8">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="G52" s="8">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="H52" s="8">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="I52" s="8">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="J52" s="8">
-        <v>1500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="53" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8818,16 +8819,16 @@
         <v>2000</v>
       </c>
       <c r="G53" s="8">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="H53" s="8">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="I53" s="8">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="J53" s="8">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8880,25 +8881,25 @@
         <v>21</v>
       </c>
       <c r="D55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="E55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="F55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="G55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="H55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="I55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="J55" s="43">
-        <v>2200</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="56" spans="1:33" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -9199,127 +9200,127 @@
       </c>
       <c r="C66" s="5">
         <f>SUMPRODUCT(D40:D56,$B$40:$B$56)/SUM($B$40:$B$56)*K$79</f>
-        <v>463.29350546214374</v>
+        <v>457.66715073896358</v>
       </c>
       <c r="D66" s="5">
         <f t="shared" ref="D66:I66" si="16">SUMPRODUCT(E40:E56,$B$40:$B$56)/SUM($B$40:$B$56)*L$79</f>
-        <v>221.09557242733794</v>
+        <v>215.72168420258612</v>
       </c>
       <c r="E66" s="5">
         <f t="shared" si="16"/>
-        <v>194.30618610622579</v>
+        <v>188.02811316670545</v>
       </c>
       <c r="F66" s="5">
         <f t="shared" si="16"/>
-        <v>255.3303083708262</v>
+        <v>181.15698643889937</v>
       </c>
       <c r="G66" s="5">
         <f t="shared" si="16"/>
-        <v>251.52892263302851</v>
+        <v>152.76346597230366</v>
       </c>
       <c r="H66" s="5">
         <f t="shared" si="16"/>
-        <v>189.20535092319807</v>
+        <v>96.20855199074947</v>
       </c>
       <c r="I66" s="5">
         <f t="shared" si="16"/>
-        <v>183.69451545941558</v>
+        <v>93.406361156067433</v>
       </c>
       <c r="J66" s="5">
         <f t="shared" ref="J66:R66" si="17">I66*R$79/Q$79</f>
-        <v>178.34418976642291</v>
+        <v>90.685787530162571</v>
       </c>
       <c r="K66" s="5">
         <f t="shared" si="17"/>
-        <v>173.14969880235233</v>
+        <v>88.04445391277919</v>
       </c>
       <c r="L66" s="5">
         <f t="shared" si="17"/>
-        <v>168.10650369160422</v>
+        <v>85.480052342504052</v>
       </c>
       <c r="M66" s="5">
         <f t="shared" si="17"/>
-        <v>163.21019775883906</v>
+        <v>82.990342080101016</v>
       </c>
       <c r="N66" s="5">
         <f t="shared" si="17"/>
-        <v>158.45650267848453</v>
+        <v>80.573147650583522</v>
       </c>
       <c r="O66" s="5">
         <f t="shared" si="17"/>
-        <v>153.8412647363927</v>
+        <v>78.226356942314084</v>
       </c>
       <c r="P66" s="5">
         <f t="shared" si="17"/>
-        <v>149.36045120038131</v>
+        <v>75.947919361469985</v>
       </c>
       <c r="Q66" s="5">
         <f t="shared" si="17"/>
-        <v>145.01014679648668</v>
+        <v>73.735844040262123</v>
       </c>
       <c r="R66" s="5">
         <f t="shared" si="17"/>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="S66" s="5">
         <f t="shared" ref="S66" si="18">R66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="T66" s="5">
         <f t="shared" ref="T66" si="19">S66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="U66" s="5">
         <f t="shared" ref="U66" si="20">T66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="V66" s="5">
         <f t="shared" ref="V66" si="21">U66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="W66" s="5">
         <f t="shared" ref="W66" si="22">V66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="X66" s="5">
         <f t="shared" ref="X66" si="23">W66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="Y66" s="5">
         <f t="shared" ref="Y66" si="24">X66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="Z66" s="5">
         <f t="shared" ref="Z66" si="25">Y66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AA66" s="5">
         <f t="shared" ref="AA66" si="26">Z66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AB66" s="5">
         <f t="shared" ref="AB66" si="27">AA66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AC66" s="5">
         <f t="shared" ref="AC66" si="28">AB66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AD66" s="5">
         <f t="shared" ref="AD66" si="29">AC66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AE66" s="5">
         <f t="shared" ref="AE66" si="30">AD66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AF66" s="5">
         <f t="shared" ref="AF66" si="31">AE66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AG66" s="5">
         <f t="shared" ref="AG66" si="32">AF66</f>
-        <v>140.78655028785116</v>
+        <v>71.588198097341873</v>
       </c>
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.35">
@@ -9425,7 +9426,7 @@
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5">
-        <f t="shared" ref="C69:AF69" si="33">B4+D65</f>
+        <f t="shared" ref="C69:AF70" si="33">B4+D65</f>
         <v>2720.1223686433941</v>
       </c>
       <c r="D69" s="5">
@@ -9550,124 +9551,124 @@
         <v>41</v>
       </c>
       <c r="C70" s="5">
-        <f t="shared" ref="C70:AF70" si="34">B5+D65</f>
-        <v>6936.9623686433943</v>
+        <f>B5+D66</f>
+        <v>6868.4416842025867</v>
       </c>
       <c r="D70" s="5">
-        <f t="shared" si="34"/>
-        <v>3848.2668213818774</v>
+        <f t="shared" si="33"/>
+        <v>3805.0781131667054</v>
       </c>
       <c r="E70" s="5">
-        <f t="shared" si="34"/>
-        <v>2129.412735209472</v>
+        <f t="shared" si="33"/>
+        <v>1976.4317864388993</v>
       </c>
       <c r="F70" s="5">
-        <f t="shared" si="34"/>
-        <v>2025.9480858626696</v>
+        <f t="shared" si="33"/>
+        <v>1914.2726659723035</v>
       </c>
       <c r="G70" s="5">
-        <f t="shared" si="34"/>
-        <v>1302.7046290858618</v>
+        <f t="shared" si="33"/>
+        <v>1198.9860519907493</v>
       </c>
       <c r="H70" s="5">
-        <f t="shared" si="34"/>
-        <v>1251.3865088212251</v>
+        <f t="shared" si="33"/>
+        <v>1150.6888611560676</v>
       </c>
       <c r="I70" s="5">
-        <f t="shared" si="34"/>
-        <v>1211.2404940011895</v>
+        <f t="shared" si="33"/>
+        <v>1113.4757875301625</v>
       </c>
       <c r="J70" s="5">
-        <f t="shared" si="34"/>
-        <v>1207.7766446613491</v>
+        <f t="shared" si="33"/>
+        <v>1112.8594539127791</v>
       </c>
       <c r="K70" s="5">
-        <f t="shared" si="34"/>
-        <v>1209.1801647197562</v>
+        <f t="shared" si="33"/>
+        <v>1117.0275523425039</v>
       </c>
       <c r="L70" s="5">
-        <f t="shared" si="34"/>
-        <v>1262.2663977861712</v>
+        <f t="shared" si="33"/>
+        <v>1172.797842080101</v>
       </c>
       <c r="M70" s="5">
-        <f t="shared" si="34"/>
-        <v>1313.0283230933701</v>
+        <f t="shared" si="33"/>
+        <v>1226.1656476505834</v>
       </c>
       <c r="N70" s="5">
-        <f t="shared" si="34"/>
-        <v>1318.9340515469612</v>
+        <f t="shared" si="33"/>
+        <v>1234.6013569423142</v>
       </c>
       <c r="O70" s="5">
-        <f t="shared" si="34"/>
-        <v>157.82432189025366</v>
+        <f t="shared" si="33"/>
+        <v>75.947919361469985</v>
       </c>
       <c r="P70" s="5">
-        <f t="shared" si="34"/>
-        <v>153.22749698082879</v>
+        <f t="shared" si="33"/>
+        <v>73.735844040262123</v>
       </c>
       <c r="Q70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="R70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="S70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="T70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="U70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="V70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="W70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="X70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="Y70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="Z70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="AA70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="AB70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="AC70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="AD70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="AE70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="AF70" s="5">
-        <f t="shared" si="34"/>
-        <v>148.76456017556194</v>
+        <f t="shared" si="33"/>
+        <v>71.588198097341873</v>
       </c>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.35">
@@ -10231,7 +10232,7 @@
         <v>0.03</v>
       </c>
       <c r="G100" s="22">
-        <f t="shared" ref="G100:G109" si="35">D$84/D100</f>
+        <f t="shared" ref="G100:G109" si="34">D$84/D100</f>
         <v>0.68990103306668438</v>
       </c>
     </row>
@@ -10246,7 +10247,7 @@
         <v>0.03</v>
       </c>
       <c r="G101" s="22">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.66980682822008197</v>
       </c>
     </row>
@@ -10261,7 +10262,7 @@
         <v>0.03</v>
       </c>
       <c r="G102" s="22">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.65029789147580774</v>
       </c>
     </row>
@@ -10276,7 +10277,7 @@
         <v>0.03</v>
       </c>
       <c r="G103" s="22">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.63135717619010456</v>
       </c>
     </row>
@@ -10291,7 +10292,7 @@
         <v>0.03</v>
       </c>
       <c r="G104" s="22">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.61296813222340252</v>
       </c>
     </row>
@@ -10306,7 +10307,7 @@
         <v>0.03</v>
       </c>
       <c r="G105" s="22">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.59511469147903162</v>
       </c>
     </row>
@@ -10321,7 +10322,7 @@
         <v>0.03</v>
       </c>
       <c r="G106" s="22">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.57778125386313739</v>
       </c>
     </row>
@@ -10336,7 +10337,7 @@
         <v>0.03</v>
       </c>
       <c r="G107" s="22">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.56095267365353152</v>
       </c>
     </row>
@@ -10351,7 +10352,7 @@
         <v>0.03</v>
       </c>
       <c r="G108" s="22">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.54461424626556454</v>
       </c>
     </row>
@@ -10366,7 +10367,7 @@
         <v>0.03</v>
       </c>
       <c r="G109" s="22">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.52875169540346068</v>
       </c>
     </row>
@@ -12788,123 +12789,123 @@
       </c>
       <c r="B6" s="18">
         <f>'Passenger Vehicle Calculations'!C70</f>
-        <v>6936.9623686433943</v>
+        <v>6868.4416842025867</v>
       </c>
       <c r="C6" s="18">
         <f>'Passenger Vehicle Calculations'!D70</f>
-        <v>3848.2668213818774</v>
+        <v>3805.0781131667054</v>
       </c>
       <c r="D6" s="18">
         <f>'Passenger Vehicle Calculations'!E70</f>
-        <v>2129.412735209472</v>
+        <v>1976.4317864388993</v>
       </c>
       <c r="E6" s="18">
         <f>'Passenger Vehicle Calculations'!F70</f>
-        <v>2025.9480858626696</v>
+        <v>1914.2726659723035</v>
       </c>
       <c r="F6" s="18">
         <f>'Passenger Vehicle Calculations'!G70</f>
-        <v>1302.7046290858618</v>
+        <v>1198.9860519907493</v>
       </c>
       <c r="G6" s="18">
         <f>'Passenger Vehicle Calculations'!H70</f>
-        <v>1251.3865088212251</v>
+        <v>1150.6888611560676</v>
       </c>
       <c r="H6" s="18">
         <f>'Passenger Vehicle Calculations'!I70</f>
-        <v>1211.2404940011895</v>
+        <v>1113.4757875301625</v>
       </c>
       <c r="I6" s="18">
         <f>'Passenger Vehicle Calculations'!J70</f>
-        <v>1207.7766446613491</v>
+        <v>1112.8594539127791</v>
       </c>
       <c r="J6" s="18">
         <f>'Passenger Vehicle Calculations'!K70</f>
-        <v>1209.1801647197562</v>
+        <v>1117.0275523425039</v>
       </c>
       <c r="K6" s="18">
         <f>'Passenger Vehicle Calculations'!L70</f>
-        <v>1262.2663977861712</v>
+        <v>1172.797842080101</v>
       </c>
       <c r="L6" s="18">
         <f>'Passenger Vehicle Calculations'!M70</f>
-        <v>1313.0283230933701</v>
+        <v>1226.1656476505834</v>
       </c>
       <c r="M6" s="18">
         <f>'Passenger Vehicle Calculations'!N70</f>
-        <v>1318.9340515469612</v>
+        <v>1234.6013569423142</v>
       </c>
       <c r="N6" s="18">
         <f>'Passenger Vehicle Calculations'!O70</f>
-        <v>157.82432189025366</v>
+        <v>75.947919361469985</v>
       </c>
       <c r="O6" s="18">
         <f>'Passenger Vehicle Calculations'!P70</f>
-        <v>153.22749698082879</v>
+        <v>73.735844040262123</v>
       </c>
       <c r="P6" s="18">
         <f>'Passenger Vehicle Calculations'!Q70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="Q6" s="18">
         <f>'Passenger Vehicle Calculations'!R70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="R6" s="18">
         <f>'Passenger Vehicle Calculations'!S70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="S6" s="18">
         <f>'Passenger Vehicle Calculations'!T70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="T6" s="18">
         <f>'Passenger Vehicle Calculations'!U70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="U6" s="18">
         <f>'Passenger Vehicle Calculations'!V70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="V6" s="18">
         <f>'Passenger Vehicle Calculations'!W70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="W6" s="18">
         <f>'Passenger Vehicle Calculations'!X70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="X6" s="18">
         <f>'Passenger Vehicle Calculations'!Y70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="Y6" s="18">
         <f>'Passenger Vehicle Calculations'!Z70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="Z6" s="18">
         <f>'Passenger Vehicle Calculations'!AA70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AA6" s="18">
         <f>'Passenger Vehicle Calculations'!AB70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AB6" s="18">
         <f>'Passenger Vehicle Calculations'!AC70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AC6" s="18">
         <f>'Passenger Vehicle Calculations'!AD70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AD6" s="18">
         <f>'Passenger Vehicle Calculations'!AE70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="AE6" s="18">
         <f>'Passenger Vehicle Calculations'!AF70</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
correcting state subsidy formula for PHEV
</commit_message>
<xml_diff>
--- a/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
+++ b/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\trans\BVS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire Trevisan\GitHub\Climate Imperative EPS repos\eps-us-ci\InputData\trans\BVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD49FB6-8DA8-4910-B887-5CA9FDF4C6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82218EA2-F539-4938-8CEB-B66A3484C6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5970" yWindow="1380" windowWidth="20940" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="123">
   <si>
     <t>Sources:</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>USA</t>
-  </si>
-  <si>
-    <t>Note: Pennsylvania offers a $1750 rebate, but only to the first 250 qualified applicants.</t>
   </si>
   <si>
     <t>Total Tax Credit (2012$)</t>
@@ -527,8 +524,8 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="167" formatCode="m\-d"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="m\-d"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -829,7 +826,7 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -866,11 +863,11 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="31" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="31" applyFont="1"/>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="31" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="31" applyFont="1"/>
@@ -885,7 +882,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="32" applyFont="1"/>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="31" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="31" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="31" applyFont="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -898,7 +895,6 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="33" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="34">
@@ -1305,69 +1301,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="69.26953125" customWidth="1"/>
+    <col min="2" max="2" width="69.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
   </sheetData>
@@ -1388,12 +1384,12 @@
       <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1488,7 +1484,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1583,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1678,7 +1674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1773,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1868,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1963,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2058,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2169,7 +2165,7 @@
       <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2186,12 +2182,12 @@
       <selection activeCell="D7" sqref="D7:M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2286,7 +2282,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2391,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2486,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2581,7 +2577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2676,7 +2672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2781,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2876,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2998,12 +2994,12 @@
       <selection activeCell="D7" sqref="D7:M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -3098,7 +3094,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3203,7 +3199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3298,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3393,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3488,7 +3484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3593,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3688,7 +3684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3809,12 +3805,12 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -3909,7 +3905,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4004,7 +4000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4099,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4194,7 +4190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4289,7 +4285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4384,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4479,7 +4475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4590,12 +4586,12 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -4690,7 +4686,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4785,7 +4781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4880,7 +4876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4975,7 +4971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5070,7 +5066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5165,7 +5161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -5260,7 +5256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -5371,12 +5367,12 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -5471,7 +5467,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5566,7 +5562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5661,7 +5657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5756,7 +5752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5851,7 +5847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5946,7 +5942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -6041,7 +6037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -6152,12 +6148,12 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -6252,7 +6248,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6347,7 +6343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6442,7 +6438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6537,7 +6533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -6632,7 +6628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -6727,7 +6723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -6822,7 +6818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -6926,38 +6922,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A3CC6-8591-4A07-9E4B-1DE39D29E87F}">
   <dimension ref="A1:AF107"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J80" sqref="J80"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.453125" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" customWidth="1"/>
-    <col min="4" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2021</v>
       </c>
@@ -7049,139 +7045,139 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="48">
+        <v>1646.4981124797289</v>
+      </c>
+      <c r="C5" s="48">
+        <v>1368.5857570401329</v>
+      </c>
+      <c r="D5" s="48">
+        <v>4795.9636566176632</v>
+      </c>
+      <c r="E5" s="48">
+        <v>3555.487701851609</v>
+      </c>
+      <c r="F5" s="48">
+        <v>3365.6876734116477</v>
+      </c>
+      <c r="G5" s="48">
+        <v>3118.2246810233032</v>
+      </c>
+      <c r="H5" s="48">
+        <v>2391.1775782482218</v>
+      </c>
+      <c r="I5" s="48">
+        <v>2424.5099210417061</v>
+      </c>
+      <c r="J5" s="48">
+        <v>2459.8873208312061</v>
+      </c>
+      <c r="K5" s="48">
+        <v>2497.1120748745493</v>
+      </c>
+      <c r="L5" s="48">
+        <v>2525.3972397122579</v>
+      </c>
+      <c r="M5" s="48">
+        <v>2552.5012628800359</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="49">
-        <v>1646.4981124797289</v>
-      </c>
-      <c r="C5" s="49">
-        <v>1368.5857570401329</v>
-      </c>
-      <c r="D5" s="49">
-        <v>4795.9636566176632</v>
-      </c>
-      <c r="E5" s="49">
-        <v>3555.487701851609</v>
-      </c>
-      <c r="F5" s="49">
-        <v>3365.6876734116477</v>
-      </c>
-      <c r="G5" s="49">
-        <v>3118.2246810233032</v>
-      </c>
-      <c r="H5" s="49">
-        <v>2391.1775782482218</v>
-      </c>
-      <c r="I5" s="49">
-        <v>2424.5099210417061</v>
-      </c>
-      <c r="J5" s="49">
-        <v>2459.8873208312061</v>
-      </c>
-      <c r="K5" s="49">
-        <v>2497.1120748745493</v>
-      </c>
-      <c r="L5" s="49">
-        <v>2525.3972397122579</v>
-      </c>
-      <c r="M5" s="49">
-        <v>2552.5012628800359</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-      <c r="AC5">
-        <v>0</v>
-      </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="49">
+      <c r="B6" s="48">
         <v>6652.7185168992282</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="48">
         <v>3617.050692978903</v>
       </c>
-      <c r="D6" s="49">
+      <c r="D6" s="48">
         <v>3481.1983222883337</v>
       </c>
-      <c r="E6" s="49">
+      <c r="E6" s="48">
         <v>2846.5223385773729</v>
       </c>
-      <c r="F6" s="49">
+      <c r="F6" s="48">
         <v>2396.2166523302549</v>
       </c>
-      <c r="G6" s="49">
+      <c r="G6" s="48">
         <v>2262.2795944248228</v>
       </c>
-      <c r="H6" s="49">
+      <c r="H6" s="48">
         <v>2133.3803923218893</v>
       </c>
-      <c r="I6" s="49">
+      <c r="I6" s="48">
         <v>2079.4479927022094</v>
       </c>
-      <c r="J6" s="49">
+      <c r="J6" s="48">
         <v>2027.1389823455879</v>
       </c>
-      <c r="K6" s="49">
+      <c r="K6" s="48">
         <v>1976.3952724267306</v>
       </c>
-      <c r="L6" s="49">
+      <c r="L6" s="48">
         <v>1926.1484722201324</v>
       </c>
-      <c r="M6" s="49">
+      <c r="M6" s="48">
         <v>1877.1377242807455</v>
       </c>
       <c r="N6">
@@ -7239,34 +7235,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
@@ -7275,7 +7271,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -7284,13 +7280,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="8"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
@@ -7328,13 +7324,13 @@
         <v>2026</v>
       </c>
       <c r="K16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L16" t="s">
         <v>82</v>
       </c>
-      <c r="L16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
         <v>21</v>
       </c>
@@ -7344,7 +7340,7 @@
       <c r="C17" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="36">
         <f>2000*D76+4000*(1-D76)</f>
         <v>3506.6</v>
       </c>
@@ -7371,10 +7367,10 @@
         <v>3500</v>
       </c>
       <c r="K17" s="36" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>23</v>
       </c>
@@ -7413,16 +7409,16 @@
         <v>470.61925821962228</v>
       </c>
       <c r="K18" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R18" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>25</v>
       </c>
@@ -7461,10 +7457,10 @@
         <v>2500</v>
       </c>
       <c r="K19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>26</v>
       </c>
@@ -7503,14 +7499,14 @@
         <v>351.62995755890529</v>
       </c>
       <c r="K20" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="L20" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="L20" s="10" t="s">
-        <v>88</v>
-      </c>
       <c r="M20" s="11"/>
     </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>27</v>
       </c>
@@ -7547,7 +7543,7 @@
       <c r="L21" s="10"/>
       <c r="M21" s="11"/>
     </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>29</v>
       </c>
@@ -7583,14 +7579,14 @@
         <v>0</v>
       </c>
       <c r="K22" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="L22" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="L22" s="10" t="s">
-        <v>90</v>
-      </c>
       <c r="M22" s="11"/>
     </row>
-    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>30</v>
       </c>
@@ -7622,12 +7618,12 @@
         <v>0</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="11"/>
     </row>
-    <row r="24" spans="1:18" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>31</v>
       </c>
@@ -7659,13 +7655,13 @@
         <v>0</v>
       </c>
       <c r="K24" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="R24" s="12"/>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="R24" s="12"/>
-    </row>
-    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="B25" s="47">
         <v>5.7169999999999996</v>
@@ -7695,10 +7691,10 @@
         <v>0</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>32</v>
       </c>
@@ -7730,7 +7726,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>33</v>
       </c>
@@ -7762,9 +7758,9 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B28" s="47">
         <f>500/10^6</f>
@@ -7795,12 +7791,12 @@
         <v>3000</v>
       </c>
       <c r="K28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="B29" s="47">
         <v>1.0940000000000001</v>
@@ -7830,7 +7826,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
@@ -7862,10 +7858,10 @@
         <v>2000</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>35</v>
       </c>
@@ -7904,13 +7900,13 @@
         <v>671.80394138453767</v>
       </c>
       <c r="K31" t="s">
+        <v>98</v>
+      </c>
+      <c r="L31" t="s">
         <v>99</v>
       </c>
-      <c r="L31" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>36</v>
       </c>
@@ -7942,10 +7938,10 @@
         <v>2200</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>37</v>
       </c>
@@ -7977,7 +7973,7 @@
       </c>
       <c r="K33" s="8"/>
     </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>38</v>
       </c>
@@ -7985,13 +7981,13 @@
         <v>329.5</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>19</v>
@@ -8027,7 +8023,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="36" t="s">
         <v>21</v>
       </c>
@@ -8067,7 +8063,7 @@
       </c>
       <c r="L37"/>
     </row>
-    <row r="38" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="36" t="s">
         <v>23</v>
       </c>
@@ -8107,7 +8103,7 @@
       </c>
       <c r="L38"/>
     </row>
-    <row r="39" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>25</v>
       </c>
@@ -8141,7 +8137,7 @@
       </c>
       <c r="L39"/>
     </row>
-    <row r="40" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>26</v>
       </c>
@@ -8181,7 +8177,7 @@
       </c>
       <c r="L40"/>
     </row>
-    <row r="41" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>27</v>
       </c>
@@ -8214,7 +8210,7 @@
       </c>
       <c r="L41"/>
     </row>
-    <row r="42" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>29</v>
       </c>
@@ -8251,7 +8247,7 @@
       </c>
       <c r="L42"/>
     </row>
-    <row r="43" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>30</v>
       </c>
@@ -8284,7 +8280,7 @@
       </c>
       <c r="L43"/>
     </row>
-    <row r="44" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>31</v>
       </c>
@@ -8317,9 +8313,9 @@
       </c>
       <c r="L44"/>
     </row>
-    <row r="45" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B45" s="7">
         <v>5.7169999999999996</v>
@@ -8350,7 +8346,7 @@
       </c>
       <c r="L45"/>
     </row>
-    <row r="46" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>32</v>
       </c>
@@ -8383,7 +8379,7 @@
       </c>
       <c r="L46"/>
     </row>
-    <row r="47" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>33</v>
       </c>
@@ -8417,9 +8413,9 @@
       </c>
       <c r="L47"/>
     </row>
-    <row r="48" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B48" s="7">
         <f>500/10^6</f>
@@ -8451,9 +8447,9 @@
       </c>
       <c r="L48"/>
     </row>
-    <row r="49" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B49" s="7">
         <v>1.0940000000000001</v>
@@ -8484,7 +8480,7 @@
       </c>
       <c r="L49"/>
     </row>
-    <row r="50" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>34</v>
       </c>
@@ -8517,7 +8513,7 @@
       </c>
       <c r="L50"/>
     </row>
-    <row r="51" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>35</v>
       </c>
@@ -8557,7 +8553,7 @@
       </c>
       <c r="L51"/>
     </row>
-    <row r="52" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>36</v>
       </c>
@@ -8590,7 +8586,7 @@
       </c>
       <c r="L52"/>
     </row>
-    <row r="53" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>37</v>
       </c>
@@ -8622,7 +8618,7 @@
       </c>
       <c r="L53"/>
     </row>
-    <row r="54" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>38</v>
       </c>
@@ -8631,11 +8627,11 @@
       </c>
       <c r="L54"/>
     </row>
-    <row r="55" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
     </row>
-    <row r="56" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -8647,31 +8643,29 @@
       <c r="I56" s="8"/>
       <c r="J56" s="7"/>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A57" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+    </row>
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B59">
         <v>0.78500000000000003</v>
       </c>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C62">
         <v>2021</v>
       </c>
@@ -8763,29 +8757,32 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="C63" s="5">
-        <f>SUMPRODUCT(E17:E33,$B$17:$B$33)/SUM($B$17:$B$33)*L79</f>
+        <f t="shared" ref="C63:H63" si="4">SUMPRODUCT(E17:E33,$B$17:$B$33)/SUM($B$17:$B$33)*L79</f>
         <v>284.24236864339406</v>
       </c>
       <c r="D63" s="5">
-        <f>SUMPRODUCT(F17:F33,$B$17:$B$33)/SUM($B$17:$B$33)*M79</f>
+        <f t="shared" si="4"/>
         <v>231.21682138187734</v>
       </c>
       <c r="E63" s="5">
-        <f>SUMPRODUCT(G17:G33,$B$17:$B$33)/SUM($B$17:$B$33)*N79</f>
+        <f t="shared" si="4"/>
         <v>334.13793520947195</v>
       </c>
       <c r="F63" s="5">
-        <f>SUMPRODUCT(H17:H33,$B$17:$B$33)/SUM($B$17:$B$33)*O79</f>
+        <f t="shared" si="4"/>
         <v>264.43888586266991</v>
       </c>
       <c r="G63" s="5">
-        <f>SUMPRODUCT(I17:I33,$B$17:$B$33)/SUM($B$17:$B$33)*P79</f>
+        <f t="shared" si="4"/>
         <v>199.92712908586196</v>
       </c>
       <c r="H63" s="5">
-        <f>SUMPRODUCT(J17:J33,$B$17:$B$33)/SUM($B$17:$B$33)*Q79</f>
+        <f t="shared" si="4"/>
         <v>194.10400882122519</v>
       </c>
       <c r="I63" s="5">
@@ -8793,35 +8790,35 @@
         <v>188.4504940011895</v>
       </c>
       <c r="J63" s="5">
-        <f t="shared" ref="J63:Q63" si="4">I63*S79/R79</f>
+        <f t="shared" ref="J63:Q63" si="5">I63*S79/R79</f>
         <v>182.96164466134903</v>
       </c>
       <c r="K63" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>177.63266471975632</v>
       </c>
       <c r="L63" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>172.45889778617118</v>
       </c>
       <c r="M63" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>167.43582309337009</v>
       </c>
       <c r="N63" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>162.55905154696123</v>
       </c>
       <c r="O63" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>157.82432189025366</v>
       </c>
       <c r="P63" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>153.22749698082879</v>
       </c>
       <c r="Q63" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>148.76456017556194</v>
       </c>
       <c r="R63" s="5">
@@ -8870,29 +8867,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="C64" s="5">
         <f>SUMPRODUCT(E37:E53,$B$37:$B$53)/SUM($B$37:$B$53)*L79</f>
         <v>215.72168420258612</v>
       </c>
       <c r="D64" s="5">
-        <f t="shared" ref="D64:H64" si="5">SUMPRODUCT(F37:F53,$B$37:$B$53)/SUM($B$37:$B$53)*M79</f>
+        <f t="shared" ref="D64:H64" si="6">SUMPRODUCT(F37:F53,$B$37:$B$53)/SUM($B$37:$B$53)*M79</f>
         <v>188.02811316670545</v>
       </c>
       <c r="E64" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>181.15698643889937</v>
       </c>
       <c r="F64" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>152.76346597230366</v>
       </c>
       <c r="G64" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>96.20855199074947</v>
       </c>
       <c r="H64" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>93.406361156067433</v>
       </c>
       <c r="I64" s="5">
@@ -8900,35 +8900,35 @@
         <v>90.685787530162571</v>
       </c>
       <c r="J64" s="5">
-        <f t="shared" ref="J64:Q64" si="6">I64*S79/R79</f>
+        <f t="shared" ref="J64:Q64" si="7">I64*S79/R79</f>
         <v>88.04445391277919</v>
       </c>
       <c r="K64" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>85.480052342504052</v>
       </c>
       <c r="L64" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>82.990342080101016</v>
       </c>
       <c r="M64" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>80.573147650583522</v>
       </c>
       <c r="N64" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78.226356942314084</v>
       </c>
       <c r="O64" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>75.947919361469985</v>
       </c>
       <c r="P64" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>73.735844040262123</v>
       </c>
       <c r="Q64" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>71.588198097341873</v>
       </c>
       <c r="R64" s="5">
@@ -8977,15 +8977,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C67">
         <v>2021</v>
       </c>
@@ -9077,260 +9077,260 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5">
-        <f>B5+C63</f>
+        <f t="shared" ref="C68:AF68" si="8">B5+C63</f>
         <v>1930.7404811231229</v>
       </c>
       <c r="D68" s="5">
-        <f>C5+D63</f>
+        <f t="shared" si="8"/>
         <v>1599.8025784220101</v>
       </c>
       <c r="E68" s="5">
-        <f>D5+E63</f>
+        <f t="shared" si="8"/>
         <v>5130.1015918271351</v>
       </c>
       <c r="F68" s="5">
-        <f>E5+F63</f>
+        <f t="shared" si="8"/>
         <v>3819.9265877142789</v>
       </c>
       <c r="G68" s="5">
-        <f>F5+G63</f>
+        <f t="shared" si="8"/>
         <v>3565.6148024975096</v>
       </c>
       <c r="H68" s="5">
-        <f>G5+H63</f>
+        <f t="shared" si="8"/>
         <v>3312.3286898445285</v>
       </c>
       <c r="I68" s="5">
-        <f>H5+I63</f>
+        <f t="shared" si="8"/>
         <v>2579.6280722494112</v>
       </c>
       <c r="J68" s="5">
-        <f>I5+J63</f>
+        <f t="shared" si="8"/>
         <v>2607.4715657030551</v>
       </c>
       <c r="K68" s="5">
-        <f>J5+K63</f>
+        <f t="shared" si="8"/>
         <v>2637.5199855509622</v>
       </c>
       <c r="L68" s="5">
-        <f>K5+L63</f>
+        <f t="shared" si="8"/>
         <v>2669.5709726607206</v>
       </c>
       <c r="M68" s="5">
-        <f>L5+M63</f>
+        <f t="shared" si="8"/>
         <v>2692.8330628056278</v>
       </c>
       <c r="N68" s="5">
-        <f>M5+N63</f>
+        <f t="shared" si="8"/>
         <v>2715.0603144269971</v>
       </c>
       <c r="O68" s="5">
-        <f>N5+O63</f>
+        <f t="shared" si="8"/>
         <v>157.82432189025366</v>
       </c>
       <c r="P68" s="5">
-        <f>O5+P63</f>
+        <f t="shared" si="8"/>
         <v>153.22749698082879</v>
       </c>
       <c r="Q68" s="5">
-        <f>P5+Q63</f>
+        <f t="shared" si="8"/>
         <v>148.76456017556194</v>
       </c>
       <c r="R68" s="5">
-        <f>Q5+R63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="S68" s="5">
-        <f>R5+S63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T68" s="5">
-        <f>S5+T63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U68" s="5">
-        <f>T5+U63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V68" s="5">
-        <f>U5+V63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W68" s="5">
-        <f>V5+W63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X68" s="5">
-        <f>W5+X63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y68" s="5">
-        <f>X5+Y63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z68" s="5">
-        <f>Y5+Z63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA68" s="5">
-        <f>Z5+AA63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AB68" s="5">
-        <f>AA5+AB63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC68" s="5">
-        <f>AB5+AC63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD68" s="5">
-        <f>AC5+AD63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE68" s="5">
-        <f>AD5+AE63</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF68" s="5">
-        <f>AE5+AF63</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.35">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C69" s="5">
-        <f>B6+C63</f>
-        <v>6936.9608855426222</v>
+        <f>B6+C64</f>
+        <v>6868.4402011018146</v>
       </c>
       <c r="D69" s="5">
-        <f>C6+D63</f>
-        <v>3848.2675143607803</v>
+        <f t="shared" ref="D69:AF69" si="9">C6+D64</f>
+        <v>3805.0788061456087</v>
       </c>
       <c r="E69" s="5">
-        <f>D6+E63</f>
-        <v>3815.3362574978055</v>
+        <f t="shared" si="9"/>
+        <v>3662.355308727233</v>
       </c>
       <c r="F69" s="5">
-        <f>E6+F63</f>
-        <v>3110.9612244400428</v>
+        <f t="shared" si="9"/>
+        <v>2999.2858045496764</v>
       </c>
       <c r="G69" s="5">
-        <f>F6+G63</f>
-        <v>2596.1437814161168</v>
+        <f t="shared" si="9"/>
+        <v>2492.4252043210045</v>
       </c>
       <c r="H69" s="5">
-        <f>G6+H63</f>
-        <v>2456.3836032460481</v>
+        <f t="shared" si="9"/>
+        <v>2355.6859555808901</v>
       </c>
       <c r="I69" s="5">
-        <f>H6+I63</f>
-        <v>2321.8308863230786</v>
+        <f t="shared" si="9"/>
+        <v>2224.0661798520518</v>
       </c>
       <c r="J69" s="5">
-        <f>I6+J63</f>
-        <v>2262.4096373635584</v>
+        <f t="shared" si="9"/>
+        <v>2167.4924466149887</v>
       </c>
       <c r="K69" s="5">
-        <f>J6+K63</f>
-        <v>2204.771647065344</v>
+        <f t="shared" si="9"/>
+        <v>2112.6190346880921</v>
       </c>
       <c r="L69" s="5">
-        <f>K6+L63</f>
-        <v>2148.8541702129019</v>
+        <f t="shared" si="9"/>
+        <v>2059.3856145068316</v>
       </c>
       <c r="M69" s="5">
-        <f>L6+M63</f>
-        <v>2093.5842953135025</v>
+        <f t="shared" si="9"/>
+        <v>2006.7216198707158</v>
       </c>
       <c r="N69" s="5">
-        <f>M6+N63</f>
-        <v>2039.6967758277067</v>
+        <f t="shared" si="9"/>
+        <v>1955.3640812230597</v>
       </c>
       <c r="O69" s="5">
-        <f>N6+O63</f>
-        <v>157.82432189025366</v>
+        <f t="shared" si="9"/>
+        <v>75.947919361469985</v>
       </c>
       <c r="P69" s="5">
-        <f>O6+P63</f>
-        <v>153.22749698082879</v>
+        <f t="shared" si="9"/>
+        <v>73.735844040262123</v>
       </c>
       <c r="Q69" s="5">
-        <f>P6+Q63</f>
-        <v>148.76456017556194</v>
+        <f t="shared" si="9"/>
+        <v>71.588198097341873</v>
       </c>
       <c r="R69" s="5">
-        <f>Q6+R63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S69" s="5">
-        <f>R6+S63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="T69" s="5">
-        <f>S6+T63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U69" s="5">
-        <f>T6+U63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V69" s="5">
-        <f>U6+V63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W69" s="5">
-        <f>V6+W63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X69" s="5">
-        <f>W6+X63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y69" s="5">
-        <f>X6+Y63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Z69" s="5">
-        <f>Y6+Z63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA69" s="5">
-        <f>Z6+AA63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AB69" s="5">
-        <f>AA6+AB63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AC69" s="5">
-        <f>AB6+AC63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AD69" s="5">
-        <f>AC6+AD63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE69" s="5">
-        <f>AD6+AE63</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF69" s="5">
-        <f>AE6+AF63</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D73" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E73" s="22"/>
       <c r="F73" s="22"/>
@@ -9339,9 +9339,9 @@
       <c r="I73" s="22"/>
       <c r="J73" s="22"/>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D74" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E74" s="22"/>
       <c r="F74" s="22"/>
@@ -9350,7 +9350,7 @@
       <c r="I74" s="22"/>
       <c r="J74" s="22"/>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D75" s="22">
         <v>2020</v>
       </c>
@@ -9373,7 +9373,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D76" s="40">
         <v>0.2467</v>
       </c>
@@ -9398,7 +9398,7 @@
         <v>0.46560000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B78" s="22"/>
       <c r="C78" s="22">
         <v>2012</v>
@@ -9473,9 +9473,9 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B79" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C79" s="43" cm="1">
         <f t="array" ref="C79:Z79">TRANSPOSE(G84:G107)</f>
@@ -9551,14 +9551,14 @@
         <v>0.52875169540346068</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B82" s="16"/>
       <c r="C82" s="17"/>
       <c r="D82" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E82" s="17"/>
       <c r="F82" s="17"/>
@@ -9571,9 +9571,9 @@
       <c r="K82" s="17"/>
       <c r="L82" s="15"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B84">
         <v>228.85</v>
@@ -9594,9 +9594,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B85">
         <v>232.36600000000001</v>
@@ -9617,9 +9617,9 @@
         <v>0.98556385942470071</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B86">
         <v>236.38399999999999</v>
@@ -9640,9 +9640,9 @@
         <v>0.96983137334414704</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B87">
         <v>236.26499999999999</v>
@@ -9663,9 +9663,9 @@
         <v>0.9686815713640794</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B88">
         <v>238.77799999999999</v>
@@ -9686,9 +9686,9 @@
         <v>0.95661376543184151</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B89">
         <v>244.07599999999999</v>
@@ -9709,9 +9709,9 @@
         <v>0.93665959530026111</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B90">
         <v>250.089</v>
@@ -9732,9 +9732,9 @@
         <v>0.9143273584567535</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B91">
         <v>254.41200000000001</v>
@@ -9755,9 +9755,9 @@
         <v>0.89805481563188172</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B92">
         <v>257.55700000000002</v>
@@ -9778,9 +9778,9 @@
         <v>0.88711067149387013</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B93">
         <v>266.23599999999999</v>
@@ -9801,9 +9801,9 @@
         <v>0.84730412960844359</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B94">
         <v>288.34699999999998</v>
@@ -9824,9 +9824,9 @@
         <v>0.78452102304761584</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B95">
         <v>302.40800000000002</v>
@@ -9841,9 +9841,9 @@
         <v>0.75350342301658668</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B96">
         <v>312.14499999999998</v>
@@ -9858,7 +9858,7 @@
         <v>0.73191600598044548</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2025</v>
       </c>
@@ -9875,7 +9875,7 @@
         <v>0.71059806405868498</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2026</v>
       </c>
@@ -9884,164 +9884,164 @@
         <v>332.79266010000003</v>
       </c>
       <c r="F98" s="16">
-        <f t="shared" ref="F98:F107" si="7">G$82</f>
+        <f t="shared" ref="F98:F107" si="10">G$82</f>
         <v>0.03</v>
       </c>
       <c r="G98" s="22">
-        <f t="shared" ref="G98:G107" si="8">D$84/D98</f>
+        <f t="shared" ref="G98:G107" si="11">D$84/D98</f>
         <v>0.68990103306668438</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2027</v>
       </c>
       <c r="D99">
-        <f t="shared" ref="D99:D107" si="9">D98*(1+F99)</f>
+        <f t="shared" ref="D99:D107" si="12">D98*(1+F99)</f>
         <v>342.77643990300004</v>
       </c>
       <c r="F99" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.03</v>
       </c>
       <c r="G99" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.66980682822008197</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2028</v>
       </c>
       <c r="D100">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>353.05973310009006</v>
       </c>
       <c r="F100" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.03</v>
       </c>
       <c r="G100" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.65029789147580774</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2029</v>
       </c>
       <c r="D101">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>363.65152509309274</v>
       </c>
       <c r="F101" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.03</v>
       </c>
       <c r="G101" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.63135717619010456</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2030</v>
       </c>
       <c r="D102">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>374.56107084588552</v>
       </c>
       <c r="F102" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.03</v>
       </c>
       <c r="G102" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.61296813222340252</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2031</v>
       </c>
       <c r="D103">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>385.79790297126209</v>
       </c>
       <c r="F103" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.03</v>
       </c>
       <c r="G103" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.59511469147903162</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2032</v>
       </c>
       <c r="D104">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>397.37184006039996</v>
       </c>
       <c r="F104" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.03</v>
       </c>
       <c r="G104" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.57778125386313739</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2033</v>
       </c>
       <c r="D105">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>409.29299526221195</v>
       </c>
       <c r="F105" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.03</v>
       </c>
       <c r="G105" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.56095267365353152</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2034</v>
       </c>
       <c r="D106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>421.57178512007829</v>
       </c>
       <c r="F106" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.03</v>
       </c>
       <c r="G106" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.54461424626556454</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2035</v>
       </c>
       <c r="D107">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>434.21893867368067</v>
       </c>
       <c r="F107" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.03</v>
       </c>
       <c r="G107" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.52875169540346068</v>
       </c>
     </row>
@@ -10064,19 +10064,19 @@
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.81640625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" style="22" customWidth="1"/>
-    <col min="5" max="38" width="7.54296875" style="22" customWidth="1"/>
-    <col min="39" max="16384" width="12.54296875" style="22"/>
+    <col min="1" max="1" width="51.85546875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="22" customWidth="1"/>
+    <col min="5" max="38" width="7.5703125" style="22" customWidth="1"/>
+    <col min="39" max="16384" width="12.5703125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -10116,9 +10116,9 @@
       <c r="AK1" s="21"/>
       <c r="AL1" s="21"/>
     </row>
-    <row r="2" spans="1:38" ht="104.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -10158,7 +10158,7 @@
       <c r="AK2" s="24"/>
       <c r="AL2" s="24"/>
     </row>
-    <row r="3" spans="1:38" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -10198,9 +10198,9 @@
       <c r="AK3" s="24"/>
       <c r="AL3" s="24"/>
     </row>
-    <row r="4" spans="1:38" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="34">
         <v>40000</v>
@@ -10242,9 +10242,9 @@
       <c r="AK4" s="24"/>
       <c r="AL4" s="24"/>
     </row>
-    <row r="5" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="34">
         <v>7500</v>
@@ -10286,7 +10286,7 @@
       <c r="AK5" s="24"/>
       <c r="AL5" s="24"/>
     </row>
-    <row r="6" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
@@ -10326,29 +10326,29 @@
       <c r="AK6" s="24"/>
       <c r="AL6" s="24"/>
     </row>
-    <row r="7" spans="1:38" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="26">
         <f>B4*$B$16*$B$14</f>
         <v>27004</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="26">
         <f>B4*B14</f>
         <v>31400</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
     </row>
-    <row r="10" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="22">
         <v>2023</v>
       </c>
@@ -10380,9 +10380,9 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="35">
         <f>C36</f>
@@ -10425,9 +10425,9 @@
         <v>10279.777009851599</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
@@ -10467,108 +10467,108 @@
       <c r="AK13" s="21"/>
       <c r="AL13" s="21"/>
     </row>
-    <row r="14" spans="1:38" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="25">
         <v>0.78500000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="25"/>
     </row>
-    <row r="16" spans="1:38" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="25">
         <v>0.86</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="25"/>
     </row>
-    <row r="18" spans="1:33" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="13" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
+    <row r="21" spans="1:33" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="25" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:33" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:33" ht="39" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
+      <c r="B22" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="C22" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="D22" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:33" ht="26" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
+      <c r="B23" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="C23" s="27" t="s">
         <v>59</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>60</v>
       </c>
       <c r="D23" s="26">
         <f>B5*B14</f>
         <v>5887.5</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="23">
         <v>3</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24" s="26">
         <f>D23</f>
         <v>5887.5</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="28">
         <v>44657</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="26">
         <f>B4*B14</f>
         <v>31400</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
@@ -10603,7 +10603,7 @@
       <c r="AF28" s="29"/>
       <c r="AG28" s="29"/>
     </row>
-    <row r="29" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="30"/>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
@@ -10638,9 +10638,9 @@
       <c r="AF29" s="29"/>
       <c r="AG29" s="29"/>
     </row>
-    <row r="30" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
@@ -10675,9 +10675,9 @@
       <c r="AF30" s="29"/>
       <c r="AG30" s="29"/>
     </row>
-    <row r="31" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" s="31">
         <v>2022</v>
@@ -10769,9 +10769,9 @@
       <c r="AE31" s="29"/>
       <c r="AF31" s="29"/>
     </row>
-    <row r="32" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32" s="32">
         <v>652.15881300000001</v>
@@ -10863,9 +10863,9 @@
       <c r="AE32" s="33"/>
       <c r="AF32" s="29"/>
     </row>
-    <row r="33" spans="1:32" ht="13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33" s="32">
         <v>252.12297100000001</v>
@@ -10957,9 +10957,9 @@
       <c r="AE33" s="33"/>
       <c r="AF33" s="29"/>
     </row>
-    <row r="34" spans="1:32" ht="13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B34" s="32">
         <v>180.61982699999999</v>
@@ -11051,9 +11051,9 @@
       <c r="AE34" s="33"/>
       <c r="AF34" s="29"/>
     </row>
-    <row r="36" spans="1:32" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B36" s="26">
         <f t="shared" ref="B36:AD36" si="1">SUMPRODUCT(B32:B34,$D$23:$D$25)/SUM(B32:B34)</f>
@@ -11172,746 +11172,746 @@
         <v>9558.932689351499</v>
       </c>
     </row>
-    <row r="37" spans="1:32" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:32" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:32" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:32" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:32" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:32" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:32" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:32" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:32" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:32" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:32" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:32" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="188" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="189" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="190" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="191" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="192" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="193" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="194" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="195" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="196" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="197" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="198" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="202" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="203" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="204" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="205" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="206" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="207" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="208" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="256" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="273" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="274" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="275" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="276" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="277" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="278" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="279" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="280" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="281" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="282" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="283" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="284" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="285" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="286" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="287" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="288" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="289" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="290" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="291" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="292" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="293" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="294" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="295" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="296" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="297" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="298" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="299" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="300" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="301" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="302" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="303" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="304" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="305" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="306" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="307" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="308" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="309" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="310" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="311" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="312" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="313" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="314" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="315" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="316" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="317" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="318" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="319" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="320" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="321" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="322" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="323" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="324" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="325" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="326" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="327" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="328" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="329" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="330" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="331" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="332" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="333" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="334" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="335" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="336" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="337" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="338" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="339" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="340" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="341" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="342" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="343" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="344" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="345" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="346" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="347" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="348" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="349" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="350" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="353" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="354" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="355" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="356" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="357" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="358" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="359" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="360" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="361" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="362" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="363" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="364" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="365" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="366" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="367" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="368" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="369" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="370" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="371" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="372" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="373" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="374" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="375" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="376" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="377" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="378" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="379" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="380" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="381" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="382" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="383" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="384" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="385" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="386" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="387" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="388" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="389" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="390" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="391" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="392" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="393" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="394" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="395" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="396" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="397" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="398" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="399" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="400" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="401" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="402" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="403" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="404" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="405" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="406" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="407" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="408" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="409" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="410" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="411" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="412" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="413" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="414" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="415" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="416" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="417" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="418" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="419" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="420" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="421" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="422" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="423" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="424" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="425" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="426" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="427" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="428" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="429" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="430" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="431" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="432" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="433" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="434" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="435" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="436" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="437" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="438" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="439" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="440" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="441" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="442" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="443" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="444" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="445" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="446" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="447" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="448" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="449" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="450" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="451" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="452" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="453" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="454" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="455" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="456" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="457" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="458" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="459" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="460" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="461" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="462" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="463" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="464" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="505" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="506" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="507" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="508" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -11929,7 +11929,7 @@
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11946,13 +11946,13 @@
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
-    <col min="2" max="2" width="53.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -12047,7 +12047,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -12172,7 +12172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -12267,7 +12267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -12362,7 +12362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -12457,69 +12457,69 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="18">
         <f>'Passenger Vehicle Calculations'!C69</f>
-        <v>6936.9608855426222</v>
+        <v>6868.4402011018146</v>
       </c>
       <c r="C6" s="18">
         <f>'Passenger Vehicle Calculations'!D69</f>
-        <v>3848.2675143607803</v>
+        <v>3805.0788061456087</v>
       </c>
       <c r="D6" s="18">
         <f>'Passenger Vehicle Calculations'!E69</f>
-        <v>3815.3362574978055</v>
+        <v>3662.355308727233</v>
       </c>
       <c r="E6" s="18">
         <f>'Passenger Vehicle Calculations'!F69</f>
-        <v>3110.9612244400428</v>
+        <v>2999.2858045496764</v>
       </c>
       <c r="F6" s="18">
         <f>'Passenger Vehicle Calculations'!G69</f>
-        <v>2596.1437814161168</v>
+        <v>2492.4252043210045</v>
       </c>
       <c r="G6" s="18">
         <f>'Passenger Vehicle Calculations'!H69</f>
-        <v>2456.3836032460481</v>
+        <v>2355.6859555808901</v>
       </c>
       <c r="H6" s="18">
         <f>'Passenger Vehicle Calculations'!I69</f>
-        <v>2321.8308863230786</v>
+        <v>2224.0661798520518</v>
       </c>
       <c r="I6" s="18">
         <f>'Passenger Vehicle Calculations'!J69</f>
-        <v>2262.4096373635584</v>
+        <v>2167.4924466149887</v>
       </c>
       <c r="J6" s="18">
         <f>'Passenger Vehicle Calculations'!K69</f>
-        <v>2204.771647065344</v>
+        <v>2112.6190346880921</v>
       </c>
       <c r="K6" s="18">
         <f>'Passenger Vehicle Calculations'!L69</f>
-        <v>2148.8541702129019</v>
+        <v>2059.3856145068316</v>
       </c>
       <c r="L6" s="18">
         <f>'Passenger Vehicle Calculations'!M69</f>
-        <v>2093.5842953135025</v>
+        <v>2006.7216198707158</v>
       </c>
       <c r="M6" s="18">
         <f>'Passenger Vehicle Calculations'!N69</f>
-        <v>2039.6967758277067</v>
+        <v>1955.3640812230597</v>
       </c>
       <c r="N6" s="18">
         <f>'Passenger Vehicle Calculations'!O69</f>
-        <v>157.82432189025366</v>
+        <v>75.947919361469985</v>
       </c>
       <c r="O6" s="18">
         <f>'Passenger Vehicle Calculations'!P69</f>
-        <v>153.22749698082879</v>
+        <v>73.735844040262123</v>
       </c>
       <c r="P6" s="18">
         <f>'Passenger Vehicle Calculations'!Q69</f>
-        <v>148.76456017556194</v>
+        <v>71.588198097341873</v>
       </c>
       <c r="Q6" s="18">
         <f>'Passenger Vehicle Calculations'!R69</f>
@@ -12582,7 +12582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -12677,7 +12677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -12817,12 +12817,12 @@
       <selection activeCell="D7" sqref="D7:M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -12917,7 +12917,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -13022,7 +13022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -13117,7 +13117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -13212,7 +13212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -13307,7 +13307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -13412,7 +13412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -13507,7 +13507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -13628,12 +13628,12 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -13728,7 +13728,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -13823,7 +13823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -13918,7 +13918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -14013,7 +14013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -14108,7 +14108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -14203,7 +14203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -14298,7 +14298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -14409,12 +14409,12 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -14509,7 +14509,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -14604,7 +14604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -14699,7 +14699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -14794,7 +14794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -14889,7 +14889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -14984,7 +14984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -15079,7 +15079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -15190,12 +15190,12 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -15290,7 +15290,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -15385,7 +15385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -15480,7 +15480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -15575,7 +15575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -15670,7 +15670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -15765,7 +15765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -15860,7 +15860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Adjusts commercial vehicle tax credits in line with inflation
</commit_message>
<xml_diff>
--- a/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
+++ b/InputData/trans/BVS/BAU Vehicle Subsidy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire Trevisan\GitHub\Climate Imperative EPS repos\eps-us-ci\InputData\trans\BVS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\trans\BVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82218EA2-F539-4938-8CEB-B66A3484C6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E25C66-036F-474A-A81B-895765D51030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -297,9 +297,6 @@
     <t>Calculations:</t>
   </si>
   <si>
-    <t>2022 $ to 2012 $</t>
-  </si>
-  <si>
     <t>Fraction of buses owned by private entities (see trans/FoVObE)</t>
   </si>
   <si>
@@ -370,9 +367,6 @@
   </si>
   <si>
     <t>Freight HDV (2012 $)</t>
-  </si>
-  <si>
-    <t>Psgr LDV (2012 $)</t>
   </si>
   <si>
     <t>Credit Amount (2012 $)</t>
@@ -515,17 +509,24 @@
   <si>
     <t>Updated 2/11/25</t>
   </si>
+  <si>
+    <t>Conversion to 2012$</t>
+  </si>
+  <si>
+    <t>Frgt LDV (2012 $)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="166" formatCode="m\-d"/>
+    <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -826,7 +827,7 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -896,6 +897,9 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="33" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="15" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="12" fillId="0" borderId="0" xfId="31" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1343,12 +1347,12 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2179,7 +2183,7 @@
   <dimension ref="A1:AE8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:M7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2293,44 +2297,44 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <f>'Commercial Vehicles'!B11</f>
-        <v>10121.162702145082</v>
+        <f>'Commercial Vehicles'!B10</f>
+        <v>9715.0710076103514</v>
       </c>
       <c r="E2">
-        <f>'Commercial Vehicles'!C11</f>
-        <v>10059.772494365814</v>
+        <f>'Commercial Vehicles'!C10</f>
+        <v>9379.5012804435319</v>
       </c>
       <c r="F2">
-        <f>'Commercial Vehicles'!D11</f>
-        <v>10050.763799597085</v>
+        <f>'Commercial Vehicles'!D10</f>
+        <v>9098.157067904207</v>
       </c>
       <c r="G2">
-        <f>'Commercial Vehicles'!E11</f>
-        <v>10127.428607069427</v>
+        <f>'Commercial Vehicles'!E10</f>
+        <v>8900.5394373583313</v>
       </c>
       <c r="H2">
-        <f>'Commercial Vehicles'!F11</f>
-        <v>10269.11524721545</v>
+        <f>'Commercial Vehicles'!F10</f>
+        <v>8762.1955571514172</v>
       </c>
       <c r="I2">
-        <f>'Commercial Vehicles'!G11</f>
-        <v>10350.781370900584</v>
+        <f>'Commercial Vehicles'!G10</f>
+        <v>8574.638599520662</v>
       </c>
       <c r="J2">
-        <f>'Commercial Vehicles'!H11</f>
-        <v>10353.674088089921</v>
+        <f>'Commercial Vehicles'!H10</f>
+        <v>8327.2183891071436</v>
       </c>
       <c r="K2">
-        <f>'Commercial Vehicles'!I11</f>
-        <v>10294.239800360298</v>
+        <f>'Commercial Vehicles'!I10</f>
+        <v>8038.2687173078502</v>
       </c>
       <c r="L2">
-        <f>'Commercial Vehicles'!J11</f>
-        <v>10251.903689786537</v>
+        <f>'Commercial Vehicles'!J10</f>
+        <v>7772.0490463949827</v>
       </c>
       <c r="M2">
-        <f>'Commercial Vehicles'!K11</f>
-        <v>10279.777009851599</v>
+        <f>'Commercial Vehicles'!K10</f>
+        <v>7566.1942040579743</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -2684,43 +2688,43 @@
       </c>
       <c r="D6">
         <f>D2</f>
-        <v>10121.162702145082</v>
+        <v>9715.0710076103514</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6:M6" si="0">E2</f>
-        <v>10059.772494365814</v>
+        <v>9379.5012804435319</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>10050.763799597085</v>
+        <v>9098.157067904207</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>10127.428607069427</v>
+        <v>8900.5394373583313</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>10269.11524721545</v>
+        <v>8762.1955571514172</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>10350.781370900584</v>
+        <v>8574.638599520662</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>10353.674088089921</v>
+        <v>8327.2183891071436</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>10294.239800360298</v>
+        <v>8038.2687173078502</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>10251.903689786537</v>
+        <v>7772.0490463949827</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>10279.777009851599</v>
+        <v>7566.1942040579743</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -2884,43 +2888,43 @@
       </c>
       <c r="D8">
         <f>D2</f>
-        <v>10121.162702145082</v>
+        <v>9715.0710076103514</v>
       </c>
       <c r="E8">
         <f t="shared" ref="E8:M8" si="1">E2</f>
-        <v>10059.772494365814</v>
+        <v>9379.5012804435319</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>10050.763799597085</v>
+        <v>9098.157067904207</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>10127.428607069427</v>
+        <v>8900.5394373583313</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>10269.11524721545</v>
+        <v>8762.1955571514172</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>10350.781370900584</v>
+        <v>8574.638599520662</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>10353.674088089921</v>
+        <v>8327.2183891071436</v>
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>10294.239800360298</v>
+        <v>8038.2687173078502</v>
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>10251.903689786537</v>
+        <v>7772.0490463949827</v>
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
-        <v>10279.777009851599</v>
+        <v>7566.1942040579743</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -2990,13 +2994,14 @@
   </sheetPr>
   <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -3104,45 +3109,45 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <f>'Commercial Vehicles'!$B$8</f>
-        <v>31400</v>
-      </c>
-      <c r="E2">
-        <f>'Commercial Vehicles'!$B$8</f>
-        <v>31400</v>
-      </c>
-      <c r="F2">
-        <f>'Commercial Vehicles'!$B$8</f>
-        <v>31400</v>
-      </c>
-      <c r="G2">
-        <f>'Commercial Vehicles'!$B$8</f>
-        <v>31400</v>
-      </c>
-      <c r="H2">
-        <f>'Commercial Vehicles'!$B$8</f>
-        <v>31400</v>
-      </c>
-      <c r="I2">
-        <f>'Commercial Vehicles'!$B$8</f>
-        <v>31400</v>
-      </c>
-      <c r="J2">
-        <f>'Commercial Vehicles'!$B$8</f>
-        <v>31400</v>
-      </c>
-      <c r="K2">
-        <f>'Commercial Vehicles'!$B$8</f>
-        <v>31400</v>
-      </c>
-      <c r="L2">
-        <f>'Commercial Vehicles'!$B$8</f>
-        <v>31400</v>
-      </c>
-      <c r="M2">
-        <f>'Commercial Vehicles'!$B$8</f>
-        <v>31400</v>
+      <c r="D2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!C14</f>
+        <v>30140.136920663466</v>
+      </c>
+      <c r="E2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!D14</f>
+        <v>29276.640239217821</v>
+      </c>
+      <c r="F2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!E14</f>
+        <v>28423.922562347398</v>
+      </c>
+      <c r="G2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!F14</f>
+        <v>27596.041322667374</v>
+      </c>
+      <c r="H2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!G14</f>
+        <v>26792.273128803277</v>
+      </c>
+      <c r="I2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!H14</f>
+        <v>26011.915659032311</v>
+      </c>
+      <c r="J2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!I14</f>
+        <v>25254.287047604183</v>
+      </c>
+      <c r="K2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!J14</f>
+        <v>24518.725288936101</v>
+      </c>
+      <c r="L2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!K14</f>
+        <v>23804.587659161265</v>
+      </c>
+      <c r="M2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!L14</f>
+        <v>23111.250154525496</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -3496,43 +3501,43 @@
       </c>
       <c r="D6">
         <f>D2</f>
-        <v>31400</v>
+        <v>30140.136920663466</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6:M6" si="0">E2</f>
-        <v>31400</v>
+        <v>29276.640239217821</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>31400</v>
+        <v>28423.922562347398</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>31400</v>
+        <v>27596.041322667374</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>31400</v>
+        <v>26792.273128803277</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>31400</v>
+        <v>26011.915659032311</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>31400</v>
+        <v>25254.287047604183</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>31400</v>
+        <v>24518.725288936101</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>31400</v>
+        <v>23804.587659161265</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>31400</v>
+        <v>23111.250154525496</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -3696,43 +3701,43 @@
       </c>
       <c r="D8">
         <f>D2</f>
-        <v>31400</v>
+        <v>30140.136920663466</v>
       </c>
       <c r="E8">
         <f t="shared" ref="E8:M8" si="1">E2</f>
-        <v>31400</v>
+        <v>29276.640239217821</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>31400</v>
+        <v>28423.922562347398</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>31400</v>
+        <v>27596.041322667374</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>31400</v>
+        <v>26792.273128803277</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>31400</v>
+        <v>26011.915659032311</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>31400</v>
+        <v>25254.287047604183</v>
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>31400</v>
+        <v>24518.725288936101</v>
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>31400</v>
+        <v>23804.587659161265</v>
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
-        <v>31400</v>
+        <v>23111.250154525496</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -6922,8 +6927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A3CC6-8591-4A07-9E4B-1DE39D29E87F}">
   <dimension ref="A1:AF107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6945,12 +6950,12 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -7258,7 +7263,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B12" s="7"/>
     </row>
@@ -7324,10 +7329,10 @@
         <v>2026</v>
       </c>
       <c r="K16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -7367,7 +7372,7 @@
         <v>3500</v>
       </c>
       <c r="K17" s="36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -7409,10 +7414,10 @@
         <v>470.61925821962228</v>
       </c>
       <c r="K18" s="36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="R18" s="9" t="s">
         <v>24</v>
@@ -7457,7 +7462,7 @@
         <v>2500</v>
       </c>
       <c r="K19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7499,10 +7504,10 @@
         <v>351.62995755890529</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M20" s="11"/>
     </row>
@@ -7579,10 +7584,10 @@
         <v>0</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M22" s="11"/>
     </row>
@@ -7618,7 +7623,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="11"/>
@@ -7655,13 +7660,13 @@
         <v>0</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R24" s="12"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B25" s="47">
         <v>5.7169999999999996</v>
@@ -7691,7 +7696,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7760,7 +7765,7 @@
     </row>
     <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B28" s="47">
         <f>500/10^6</f>
@@ -7791,12 +7796,12 @@
         <v>3000</v>
       </c>
       <c r="K28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B29" s="47">
         <v>1.0940000000000001</v>
@@ -7858,7 +7863,7 @@
         <v>2000</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7900,10 +7905,10 @@
         <v>671.80394138453767</v>
       </c>
       <c r="K31" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L31" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7938,7 +7943,7 @@
         <v>2200</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7987,7 +7992,7 @@
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>19</v>
@@ -8315,7 +8320,7 @@
     </row>
     <row r="45" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B45" s="7">
         <v>5.7169999999999996</v>
@@ -8415,7 +8420,7 @@
     </row>
     <row r="48" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B48" s="7">
         <f>500/10^6</f>
@@ -8449,7 +8454,7 @@
     </row>
     <row r="49" spans="1:32" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B49" s="7">
         <v>1.0940000000000001</v>
@@ -9330,7 +9335,7 @@
     </row>
     <row r="73" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D73" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E73" s="22"/>
       <c r="F73" s="22"/>
@@ -9341,7 +9346,7 @@
     </row>
     <row r="74" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D74" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E74" s="22"/>
       <c r="F74" s="22"/>
@@ -9475,7 +9480,7 @@
     </row>
     <row r="79" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B79" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C79" s="43" cm="1">
         <f t="array" ref="C79:Z79">TRANSPOSE(G84:G107)</f>
@@ -9553,12 +9558,12 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B82" s="16"/>
       <c r="C82" s="17"/>
       <c r="D82" s="17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E82" s="17"/>
       <c r="F82" s="17"/>
@@ -9573,7 +9578,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B84">
         <v>228.85</v>
@@ -9596,7 +9601,7 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B85">
         <v>232.36600000000001</v>
@@ -9619,7 +9624,7 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B86">
         <v>236.38399999999999</v>
@@ -9642,7 +9647,7 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B87">
         <v>236.26499999999999</v>
@@ -9665,7 +9670,7 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B88">
         <v>238.77799999999999</v>
@@ -9688,7 +9693,7 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B89">
         <v>244.07599999999999</v>
@@ -9711,7 +9716,7 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B90">
         <v>250.089</v>
@@ -9734,7 +9739,7 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B91">
         <v>254.41200000000001</v>
@@ -9757,7 +9762,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B92">
         <v>257.55700000000002</v>
@@ -9780,7 +9785,7 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B93">
         <v>266.23599999999999</v>
@@ -9803,7 +9808,7 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B94">
         <v>288.34699999999998</v>
@@ -9826,7 +9831,7 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B95">
         <v>302.40800000000002</v>
@@ -9843,7 +9848,7 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B96">
         <v>312.14499999999998</v>
@@ -10061,7 +10066,7 @@
   <dimension ref="A1:AL776"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10118,7 +10123,7 @@
     </row>
     <row r="2" spans="1:38" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -10200,7 +10205,7 @@
     </row>
     <row r="4" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="34">
         <v>40000</v>
@@ -10244,7 +10249,7 @@
     </row>
     <row r="5" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="34">
         <v>7500</v>
@@ -10326,153 +10331,287 @@
       <c r="AK6" s="24"/>
       <c r="AL6" s="24"/>
     </row>
-    <row r="7" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="26">
-        <f>B4*$B$16*$B$14</f>
-        <v>27004</v>
+    <row r="7" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="22">
+        <v>2023</v>
+      </c>
+      <c r="C7" s="22">
+        <v>2024</v>
+      </c>
+      <c r="D7" s="22">
+        <v>2025</v>
+      </c>
+      <c r="E7" s="22">
+        <v>2026</v>
+      </c>
+      <c r="F7" s="22">
+        <v>2027</v>
+      </c>
+      <c r="G7" s="22">
+        <v>2028</v>
+      </c>
+      <c r="H7" s="22">
+        <v>2029</v>
+      </c>
+      <c r="I7" s="22">
+        <v>2030</v>
+      </c>
+      <c r="J7" s="22">
+        <v>2031</v>
+      </c>
+      <c r="K7" s="22">
+        <v>2032</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" s="26">
-        <f>B4*B14</f>
-        <v>31400</v>
+        <f>$B4*$B$16*C$14</f>
+        <v>25920.517751770582</v>
+      </c>
+      <c r="C8" s="26">
+        <f>$B4*$B$16*D$14</f>
+        <v>25177.910605727324</v>
+      </c>
+      <c r="D8" s="26">
+        <f>$B4*$B$16*E$14</f>
+        <v>24444.573403618764</v>
+      </c>
+      <c r="E8" s="26">
+        <f>$B4*$B$16*F$14</f>
+        <v>23732.595537493944</v>
+      </c>
+      <c r="F8" s="26">
+        <f>$B4*$B$16*G$14</f>
+        <v>23041.354890770821</v>
+      </c>
+      <c r="G8" s="26">
+        <f>$B4*$B$16*H$14</f>
+        <v>22370.247466767785</v>
+      </c>
+      <c r="H8" s="26">
+        <f>$B4*$B$16*I$14</f>
+        <v>21718.686860939597</v>
+      </c>
+      <c r="I8" s="26">
+        <f>$B4*$B$16*J$14</f>
+        <v>21086.103748485046</v>
+      </c>
+      <c r="J8" s="26">
+        <f>$B4*$B$16*K$14</f>
+        <v>20471.945386878688</v>
+      </c>
+      <c r="K8" s="26">
+        <f>$B4*$B$16*L$14</f>
+        <v>19875.675132891927</v>
       </c>
     </row>
     <row r="9" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="26">
+        <f>$B$4*C14</f>
+        <v>30140.136920663466</v>
+      </c>
+      <c r="C9" s="26">
+        <f t="shared" ref="C9:K9" si="0">$B$4*D14</f>
+        <v>29276.640239217821</v>
+      </c>
+      <c r="D9" s="26">
+        <f t="shared" si="0"/>
+        <v>28423.922562347398</v>
+      </c>
+      <c r="E9" s="26">
+        <f t="shared" si="0"/>
+        <v>27596.041322667374</v>
+      </c>
+      <c r="F9" s="26">
+        <f t="shared" si="0"/>
+        <v>26792.273128803277</v>
+      </c>
+      <c r="G9" s="26">
+        <f t="shared" si="0"/>
+        <v>26011.915659032311</v>
+      </c>
+      <c r="H9" s="26">
+        <f t="shared" si="0"/>
+        <v>25254.287047604183</v>
+      </c>
+      <c r="I9" s="26">
+        <f t="shared" si="0"/>
+        <v>24518.725288936101</v>
+      </c>
+      <c r="J9" s="26">
+        <f t="shared" si="0"/>
+        <v>23804.587659161265</v>
+      </c>
+      <c r="K9" s="26">
+        <f t="shared" si="0"/>
+        <v>23111.250154525496</v>
+      </c>
     </row>
     <row r="10" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="22">
+      <c r="A10" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="35">
+        <f>C36</f>
+        <v>9715.0710076103514</v>
+      </c>
+      <c r="C10" s="35">
+        <f t="shared" ref="C10:K10" si="1">D36</f>
+        <v>9379.5012804435319</v>
+      </c>
+      <c r="D10" s="35">
+        <f t="shared" si="1"/>
+        <v>9098.157067904207</v>
+      </c>
+      <c r="E10" s="35">
+        <f t="shared" si="1"/>
+        <v>8900.5394373583313</v>
+      </c>
+      <c r="F10" s="35">
+        <f t="shared" si="1"/>
+        <v>8762.1955571514172</v>
+      </c>
+      <c r="G10" s="35">
+        <f t="shared" si="1"/>
+        <v>8574.638599520662</v>
+      </c>
+      <c r="H10" s="35">
+        <f t="shared" si="1"/>
+        <v>8327.2183891071436</v>
+      </c>
+      <c r="I10" s="35">
+        <f t="shared" si="1"/>
+        <v>8038.2687173078502</v>
+      </c>
+      <c r="J10" s="35">
+        <f t="shared" si="1"/>
+        <v>7772.0490463949827</v>
+      </c>
+      <c r="K10" s="35">
+        <f t="shared" si="1"/>
+        <v>7566.1942040579743</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="21"/>
+      <c r="Z12" s="21"/>
+      <c r="AA12" s="21"/>
+      <c r="AB12" s="21"/>
+      <c r="AC12" s="21"/>
+      <c r="AD12" s="21"/>
+      <c r="AE12" s="21"/>
+      <c r="AF12" s="21"/>
+      <c r="AG12" s="21"/>
+      <c r="AH12" s="21"/>
+      <c r="AI12" s="21"/>
+      <c r="AJ12" s="21"/>
+      <c r="AK12" s="21"/>
+      <c r="AL12" s="21"/>
+    </row>
+    <row r="13" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="25">
+        <v>2022</v>
+      </c>
+      <c r="C13" s="22">
         <v>2023</v>
       </c>
-      <c r="C10" s="22">
+      <c r="D13" s="25">
         <v>2024</v>
       </c>
-      <c r="D10" s="22">
+      <c r="E13" s="22">
         <v>2025</v>
       </c>
-      <c r="E10" s="22">
+      <c r="F13" s="25">
         <v>2026</v>
       </c>
-      <c r="F10" s="22">
+      <c r="G13" s="22">
         <v>2027</v>
       </c>
-      <c r="G10" s="22">
+      <c r="H13" s="25">
         <v>2028</v>
       </c>
-      <c r="H10" s="22">
+      <c r="I13" s="22">
         <v>2029</v>
       </c>
-      <c r="I10" s="22">
+      <c r="J13" s="25">
         <v>2030</v>
       </c>
-      <c r="J10" s="22">
+      <c r="K13" s="22">
         <v>2031</v>
       </c>
-      <c r="K10" s="22">
+      <c r="L13" s="25">
         <v>2032</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="35">
-        <f>C36</f>
-        <v>10121.162702145082</v>
-      </c>
-      <c r="C11" s="35">
-        <f t="shared" ref="C11:K11" si="0">D36</f>
-        <v>10059.772494365814</v>
-      </c>
-      <c r="D11" s="35">
-        <f t="shared" si="0"/>
-        <v>10050.763799597085</v>
-      </c>
-      <c r="E11" s="35">
-        <f t="shared" si="0"/>
-        <v>10127.428607069427</v>
-      </c>
-      <c r="F11" s="35">
-        <f t="shared" si="0"/>
-        <v>10269.11524721545</v>
-      </c>
-      <c r="G11" s="35">
-        <f t="shared" si="0"/>
-        <v>10350.781370900584</v>
-      </c>
-      <c r="H11" s="35">
-        <f t="shared" si="0"/>
-        <v>10353.674088089921</v>
-      </c>
-      <c r="I11" s="35">
-        <f t="shared" si="0"/>
-        <v>10294.239800360298</v>
-      </c>
-      <c r="J11" s="35">
-        <f t="shared" si="0"/>
-        <v>10251.903689786537</v>
-      </c>
-      <c r="K11" s="35">
-        <f t="shared" si="0"/>
-        <v>10279.777009851599</v>
-      </c>
-    </row>
-    <row r="13" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="21"/>
-      <c r="Y13" s="21"/>
-      <c r="Z13" s="21"/>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="21"/>
-      <c r="AC13" s="21"/>
-      <c r="AD13" s="21"/>
-      <c r="AE13" s="21"/>
-      <c r="AF13" s="21"/>
-      <c r="AG13" s="21"/>
-      <c r="AH13" s="21"/>
-      <c r="AI13" s="21"/>
-      <c r="AJ13" s="21"/>
-      <c r="AK13" s="21"/>
-      <c r="AL13" s="21"/>
-    </row>
     <row r="14" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="25">
-        <v>0.78500000000000003</v>
+      <c r="A14" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="49" cm="1">
+        <f t="array" ref="B14:L14">TRANSPOSE('Passenger Vehicle Calculations'!G94:G104)</f>
+        <v>0.78452102304761584</v>
+      </c>
+      <c r="C14" s="50">
+        <v>0.75350342301658668</v>
+      </c>
+      <c r="D14" s="50">
+        <v>0.73191600598044548</v>
+      </c>
+      <c r="E14" s="50">
+        <v>0.71059806405868498</v>
+      </c>
+      <c r="F14" s="50">
+        <v>0.68990103306668438</v>
+      </c>
+      <c r="G14" s="50">
+        <v>0.66980682822008197</v>
+      </c>
+      <c r="H14" s="50">
+        <v>0.65029789147580774</v>
+      </c>
+      <c r="I14" s="50">
+        <v>0.63135717619010456</v>
+      </c>
+      <c r="J14" s="50">
+        <v>0.61296813222340252</v>
+      </c>
+      <c r="K14" s="50">
+        <v>0.59511469147903162</v>
+      </c>
+      <c r="L14" s="50">
+        <v>0.57778125386313739</v>
       </c>
     </row>
     <row r="15" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
@@ -10480,7 +10619,7 @@
     </row>
     <row r="16" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="25">
         <v>0.86</v>
@@ -10492,83 +10631,83 @@
     <row r="18" spans="1:33" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:33" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="C22" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="25" t="s">
-        <v>56</v>
-      </c>
       <c r="D22" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="C23" s="27" t="s">
         <v>58</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>59</v>
       </c>
       <c r="D23" s="26">
         <f>B5*B14</f>
-        <v>5887.5</v>
+        <v>5883.907672857119</v>
       </c>
     </row>
     <row r="24" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="23">
         <v>3</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24" s="26">
         <f>D23</f>
-        <v>5887.5</v>
+        <v>5883.907672857119</v>
       </c>
     </row>
     <row r="25" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="28">
         <v>44657</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25" s="26">
         <f>B4*B14</f>
-        <v>31400</v>
+        <v>31380.840921904633</v>
       </c>
     </row>
     <row r="26" spans="1:33" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
@@ -10640,7 +10779,7 @@
     </row>
     <row r="30" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
@@ -10677,7 +10816,7 @@
     </row>
     <row r="31" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B31" s="31">
         <v>2022</v>
@@ -10712,66 +10851,30 @@
       <c r="L31" s="31">
         <v>2032</v>
       </c>
-      <c r="M31" s="31">
-        <v>2033</v>
-      </c>
-      <c r="N31" s="31">
-        <v>2034</v>
-      </c>
-      <c r="O31" s="31">
-        <v>2035</v>
-      </c>
-      <c r="P31" s="31">
-        <v>2036</v>
-      </c>
-      <c r="Q31" s="31">
-        <v>2037</v>
-      </c>
-      <c r="R31" s="31">
-        <v>2038</v>
-      </c>
-      <c r="S31" s="31">
-        <v>2039</v>
-      </c>
-      <c r="T31" s="31">
-        <v>2040</v>
-      </c>
-      <c r="U31" s="31">
-        <v>2041</v>
-      </c>
-      <c r="V31" s="31">
-        <v>2042</v>
-      </c>
-      <c r="W31" s="31">
-        <v>2043</v>
-      </c>
-      <c r="X31" s="31">
-        <v>2044</v>
-      </c>
-      <c r="Y31" s="31">
-        <v>2045</v>
-      </c>
-      <c r="Z31" s="31">
-        <v>2046</v>
-      </c>
-      <c r="AA31" s="31">
-        <v>2047</v>
-      </c>
-      <c r="AB31" s="31">
-        <v>2048</v>
-      </c>
-      <c r="AC31" s="31">
-        <v>2049</v>
-      </c>
-      <c r="AD31" s="31">
-        <v>2050</v>
-      </c>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="31"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="31"/>
+      <c r="R31" s="31"/>
+      <c r="S31" s="31"/>
+      <c r="T31" s="31"/>
+      <c r="U31" s="31"/>
+      <c r="V31" s="31"/>
+      <c r="W31" s="31"/>
+      <c r="X31" s="31"/>
+      <c r="Y31" s="31"/>
+      <c r="Z31" s="31"/>
+      <c r="AA31" s="31"/>
+      <c r="AB31" s="31"/>
+      <c r="AC31" s="31"/>
+      <c r="AD31" s="31"/>
       <c r="AE31" s="29"/>
       <c r="AF31" s="29"/>
     </row>
     <row r="32" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B32" s="32">
         <v>652.15881300000001</v>
@@ -10806,66 +10909,30 @@
       <c r="L32" s="32">
         <v>675.92620799999997</v>
       </c>
-      <c r="M32" s="32">
-        <v>676.86370799999997</v>
-      </c>
-      <c r="N32" s="32">
-        <v>681.45581100000004</v>
-      </c>
-      <c r="O32" s="32">
-        <v>687.30078100000003</v>
-      </c>
-      <c r="P32" s="32">
-        <v>692.37145999999996</v>
-      </c>
-      <c r="Q32" s="32">
-        <v>698.31860400000005</v>
-      </c>
-      <c r="R32" s="32">
-        <v>703.59320100000002</v>
-      </c>
-      <c r="S32" s="32">
-        <v>709.57092299999999</v>
-      </c>
-      <c r="T32" s="32">
-        <v>711.90655500000003</v>
-      </c>
-      <c r="U32" s="32">
-        <v>714.37567100000001</v>
-      </c>
-      <c r="V32" s="32">
-        <v>716.10638400000005</v>
-      </c>
-      <c r="W32" s="32">
-        <v>717.97564699999998</v>
-      </c>
-      <c r="X32" s="32">
-        <v>723.98962400000005</v>
-      </c>
-      <c r="Y32" s="32">
-        <v>729.19946300000004</v>
-      </c>
-      <c r="Z32" s="32">
-        <v>732.66320800000005</v>
-      </c>
-      <c r="AA32" s="32">
-        <v>734.38165300000003</v>
-      </c>
-      <c r="AB32" s="32">
-        <v>739.21014400000001</v>
-      </c>
-      <c r="AC32" s="32">
-        <v>745.07336399999997</v>
-      </c>
-      <c r="AD32" s="32">
-        <v>1035.5</v>
-      </c>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
+      <c r="Q32" s="32"/>
+      <c r="R32" s="32"/>
+      <c r="S32" s="32"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="32"/>
+      <c r="V32" s="32"/>
+      <c r="W32" s="32"/>
+      <c r="X32" s="32"/>
+      <c r="Y32" s="32"/>
+      <c r="Z32" s="32"/>
+      <c r="AA32" s="32"/>
+      <c r="AB32" s="32"/>
+      <c r="AC32" s="32"/>
+      <c r="AD32" s="32"/>
       <c r="AE32" s="33"/>
       <c r="AF32" s="29"/>
     </row>
     <row r="33" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="32">
         <v>252.12297100000001</v>
@@ -10900,66 +10967,30 @@
       <c r="L33" s="32">
         <v>303.257294</v>
       </c>
-      <c r="M33" s="32">
-        <v>305.71603399999998</v>
-      </c>
-      <c r="N33" s="32">
-        <v>309.26257299999997</v>
-      </c>
-      <c r="O33" s="32">
-        <v>314.79812600000002</v>
-      </c>
-      <c r="P33" s="32">
-        <v>321.14746100000002</v>
-      </c>
-      <c r="Q33" s="32">
-        <v>327.09249899999998</v>
-      </c>
-      <c r="R33" s="32">
-        <v>333.56478900000002</v>
-      </c>
-      <c r="S33" s="32">
-        <v>339.75351000000001</v>
-      </c>
-      <c r="T33" s="32">
-        <v>346.38189699999998</v>
-      </c>
-      <c r="U33" s="32">
-        <v>351.209137</v>
-      </c>
-      <c r="V33" s="32">
-        <v>355.95761099999999</v>
-      </c>
-      <c r="W33" s="32">
-        <v>360.42837500000002</v>
-      </c>
-      <c r="X33" s="32">
-        <v>364.902466</v>
-      </c>
-      <c r="Y33" s="32">
-        <v>371.72610500000002</v>
-      </c>
-      <c r="Z33" s="32">
-        <v>378.28823899999998</v>
-      </c>
-      <c r="AA33" s="32">
-        <v>383.89129600000001</v>
-      </c>
-      <c r="AB33" s="32">
-        <v>388.47567700000002</v>
-      </c>
-      <c r="AC33" s="32">
-        <v>394.81222500000001</v>
-      </c>
-      <c r="AD33" s="32">
-        <v>401.96115099999997</v>
-      </c>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="32"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="32"/>
+      <c r="W33" s="32"/>
+      <c r="X33" s="32"/>
+      <c r="Y33" s="32"/>
+      <c r="Z33" s="32"/>
+      <c r="AA33" s="32"/>
+      <c r="AB33" s="32"/>
+      <c r="AC33" s="32"/>
+      <c r="AD33" s="32"/>
       <c r="AE33" s="33"/>
       <c r="AF33" s="29"/>
     </row>
     <row r="34" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="32">
         <v>180.61982699999999</v>
@@ -10994,183 +11025,93 @@
       <c r="L34" s="32">
         <v>203.63635300000001</v>
       </c>
-      <c r="M34" s="32">
-        <v>206.92961099999999</v>
-      </c>
-      <c r="N34" s="32">
-        <v>209.69859299999999</v>
-      </c>
-      <c r="O34" s="32">
-        <v>212.967072</v>
-      </c>
-      <c r="P34" s="32">
-        <v>216.125214</v>
-      </c>
-      <c r="Q34" s="32">
-        <v>219.188492</v>
-      </c>
-      <c r="R34" s="32">
-        <v>221.84333799999999</v>
-      </c>
-      <c r="S34" s="32">
-        <v>224.323059</v>
-      </c>
-      <c r="T34" s="32">
-        <v>227.32418799999999</v>
-      </c>
-      <c r="U34" s="32">
-        <v>230.371872</v>
-      </c>
-      <c r="V34" s="32">
-        <v>232.498154</v>
-      </c>
-      <c r="W34" s="32">
-        <v>235.21517900000001</v>
-      </c>
-      <c r="X34" s="32">
-        <v>236.05999800000001</v>
-      </c>
-      <c r="Y34" s="32">
-        <v>234.92872600000001</v>
-      </c>
-      <c r="Z34" s="32">
-        <v>234.37702899999999</v>
-      </c>
-      <c r="AA34" s="32">
-        <v>235.44674699999999</v>
-      </c>
-      <c r="AB34" s="32">
-        <v>237.52796900000001</v>
-      </c>
-      <c r="AC34" s="32">
-        <v>239.052933</v>
-      </c>
-      <c r="AD34" s="32">
-        <v>241.633881</v>
-      </c>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
+      <c r="P34" s="32"/>
+      <c r="Q34" s="32"/>
+      <c r="R34" s="32"/>
+      <c r="S34" s="32"/>
+      <c r="T34" s="32"/>
+      <c r="U34" s="32"/>
+      <c r="V34" s="32"/>
+      <c r="W34" s="32"/>
+      <c r="X34" s="32"/>
+      <c r="Y34" s="32"/>
+      <c r="Z34" s="32"/>
+      <c r="AA34" s="32"/>
+      <c r="AB34" s="32"/>
+      <c r="AC34" s="32"/>
+      <c r="AD34" s="32"/>
       <c r="AE34" s="33"/>
       <c r="AF34" s="29"/>
     </row>
     <row r="36" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B36" s="26">
-        <f t="shared" ref="B36:AD36" si="1">SUMPRODUCT(B32:B34,$D$23:$D$25)/SUM(B32:B34)</f>
-        <v>10134.948146095066</v>
+        <f t="shared" ref="B36:AD36" si="2">SUMPRODUCT(B32:B34,$D$23:$D$25)/SUM(B32:B34)</f>
+        <v>10128.764188673933</v>
       </c>
       <c r="C36" s="26">
-        <f t="shared" si="1"/>
-        <v>10121.162702145082</v>
+        <f>SUMPRODUCT(C32:C34,$D$23:$D$25)/SUM(C32:C34)*C14/$B$14</f>
+        <v>9715.0710076103514</v>
       </c>
       <c r="D36" s="26">
-        <f t="shared" si="1"/>
-        <v>10059.772494365814</v>
+        <f t="shared" ref="D36:L36" si="3">SUMPRODUCT(D32:D34,$D$23:$D$25)/SUM(D32:D34)*D14/$B$14</f>
+        <v>9379.5012804435319</v>
       </c>
       <c r="E36" s="26">
-        <f t="shared" si="1"/>
-        <v>10050.763799597085</v>
+        <f t="shared" si="3"/>
+        <v>9098.157067904207</v>
       </c>
       <c r="F36" s="26">
-        <f t="shared" si="1"/>
-        <v>10127.428607069427</v>
+        <f t="shared" si="3"/>
+        <v>8900.5394373583313</v>
       </c>
       <c r="G36" s="26">
-        <f t="shared" si="1"/>
-        <v>10269.11524721545</v>
+        <f t="shared" si="3"/>
+        <v>8762.1955571514172</v>
       </c>
       <c r="H36" s="26">
-        <f t="shared" si="1"/>
-        <v>10350.781370900584</v>
+        <f t="shared" si="3"/>
+        <v>8574.638599520662</v>
       </c>
       <c r="I36" s="26">
-        <f t="shared" si="1"/>
-        <v>10353.674088089921</v>
+        <f t="shared" si="3"/>
+        <v>8327.2183891071436</v>
       </c>
       <c r="J36" s="26">
-        <f t="shared" si="1"/>
-        <v>10294.239800360298</v>
+        <f t="shared" si="3"/>
+        <v>8038.2687173078502</v>
       </c>
       <c r="K36" s="26">
-        <f t="shared" si="1"/>
-        <v>10251.903689786537</v>
+        <f t="shared" si="3"/>
+        <v>7772.0490463949827</v>
       </c>
       <c r="L36" s="26">
-        <f t="shared" si="1"/>
-        <v>10279.777009851599</v>
-      </c>
-      <c r="M36" s="26">
-        <f t="shared" si="1"/>
-        <v>10325.709491436844</v>
-      </c>
-      <c r="N36" s="26">
-        <f t="shared" si="1"/>
-        <v>10344.230833049938</v>
-      </c>
-      <c r="O36" s="26">
-        <f t="shared" si="1"/>
-        <v>10359.12748221428</v>
-      </c>
-      <c r="P36" s="26">
-        <f t="shared" si="1"/>
-        <v>10371.638430973771</v>
-      </c>
-      <c r="Q36" s="26">
-        <f t="shared" si="1"/>
-        <v>10380.548547191598</v>
-      </c>
-      <c r="R36" s="26">
-        <f t="shared" si="1"/>
-        <v>10382.950508948947</v>
-      </c>
-      <c r="S36" s="26">
-        <f t="shared" si="1"/>
-        <v>10380.927010758403</v>
-      </c>
-      <c r="T36" s="26">
-        <f t="shared" si="1"/>
-        <v>10398.663134138134</v>
-      </c>
-      <c r="U36" s="26">
-        <f t="shared" si="1"/>
-        <v>10422.653431517481</v>
-      </c>
-      <c r="V36" s="26">
-        <f t="shared" si="1"/>
-        <v>10434.319910781423</v>
-      </c>
-      <c r="W36" s="26">
-        <f t="shared" si="1"/>
-        <v>10455.739600691937</v>
-      </c>
-      <c r="X36" s="26">
-        <f t="shared" si="1"/>
-        <v>10432.932814907192</v>
-      </c>
-      <c r="Y36" s="26">
-        <f t="shared" si="1"/>
-        <v>10374.231186923143</v>
-      </c>
-      <c r="Z36" s="26">
-        <f t="shared" si="1"/>
-        <v>10332.172107247137</v>
-      </c>
-      <c r="AA36" s="26">
-        <f t="shared" si="1"/>
-        <v>10324.781329795693</v>
-      </c>
-      <c r="AB36" s="26">
-        <f t="shared" si="1"/>
-        <v>10326.315629830769</v>
-      </c>
-      <c r="AC36" s="26">
-        <f t="shared" si="1"/>
-        <v>10310.34979051626</v>
-      </c>
-      <c r="AD36" s="26">
-        <f t="shared" si="1"/>
-        <v>9558.932689351499</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>7566.1942040579743</v>
+      </c>
+      <c r="M36" s="26"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="26"/>
+      <c r="Q36" s="26"/>
+      <c r="R36" s="26"/>
+      <c r="S36" s="26"/>
+      <c r="T36" s="26"/>
+      <c r="U36" s="26"/>
+      <c r="V36" s="26"/>
+      <c r="W36" s="26"/>
+      <c r="X36" s="26"/>
+      <c r="Y36" s="26"/>
+      <c r="Z36" s="26"/>
+      <c r="AA36" s="26"/>
+      <c r="AB36" s="26"/>
+      <c r="AC36" s="26"/>
+      <c r="AD36" s="26"/>
     </row>
     <row r="37" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:32" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -12814,12 +12755,13 @@
   <dimension ref="A1:AE8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:M7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -12927,45 +12869,45 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <f>'Commercial Vehicles'!$B$7</f>
-        <v>27004</v>
-      </c>
-      <c r="E2">
-        <f>'Commercial Vehicles'!$B$7</f>
-        <v>27004</v>
-      </c>
-      <c r="F2">
-        <f>'Commercial Vehicles'!$B$7</f>
-        <v>27004</v>
-      </c>
-      <c r="G2">
-        <f>'Commercial Vehicles'!$B$7</f>
-        <v>27004</v>
-      </c>
-      <c r="H2">
-        <f>'Commercial Vehicles'!$B$7</f>
-        <v>27004</v>
-      </c>
-      <c r="I2">
-        <f>'Commercial Vehicles'!$B$7</f>
-        <v>27004</v>
-      </c>
-      <c r="J2">
-        <f>'Commercial Vehicles'!$B$7</f>
-        <v>27004</v>
-      </c>
-      <c r="K2">
-        <f>'Commercial Vehicles'!$B$7</f>
-        <v>27004</v>
-      </c>
-      <c r="L2">
-        <f>'Commercial Vehicles'!$B$7</f>
-        <v>27004</v>
-      </c>
-      <c r="M2">
-        <f>'Commercial Vehicles'!$B$7</f>
-        <v>27004</v>
+      <c r="D2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!C14*'Commercial Vehicles'!$B16</f>
+        <v>25920.517751770582</v>
+      </c>
+      <c r="E2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!D14*'Commercial Vehicles'!$B16</f>
+        <v>25177.910605727324</v>
+      </c>
+      <c r="F2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!E14*'Commercial Vehicles'!$B16</f>
+        <v>24444.57340361876</v>
+      </c>
+      <c r="G2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!F14*'Commercial Vehicles'!$B16</f>
+        <v>23732.59553749394</v>
+      </c>
+      <c r="H2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!G14*'Commercial Vehicles'!$B16</f>
+        <v>23041.354890770817</v>
+      </c>
+      <c r="I2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!H14*'Commercial Vehicles'!$B16</f>
+        <v>22370.247466767789</v>
+      </c>
+      <c r="J2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!I14*'Commercial Vehicles'!$B16</f>
+        <v>21718.686860939597</v>
+      </c>
+      <c r="K2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!J14*'Commercial Vehicles'!$B16</f>
+        <v>21086.103748485046</v>
+      </c>
+      <c r="L2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!K14*'Commercial Vehicles'!$B16</f>
+        <v>20471.945386878688</v>
+      </c>
+      <c r="M2" s="51">
+        <f>'Commercial Vehicles'!$B4*'Commercial Vehicles'!L14*'Commercial Vehicles'!$B16</f>
+        <v>19875.675132891927</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -13319,43 +13261,43 @@
       </c>
       <c r="D6">
         <f>D2</f>
-        <v>27004</v>
+        <v>25920.517751770582</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6:M6" si="0">E2</f>
-        <v>27004</v>
+        <v>25177.910605727324</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>27004</v>
+        <v>24444.57340361876</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>27004</v>
+        <v>23732.59553749394</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>27004</v>
+        <v>23041.354890770817</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>27004</v>
+        <v>22370.247466767789</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>27004</v>
+        <v>21718.686860939597</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>27004</v>
+        <v>21086.103748485046</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>27004</v>
+        <v>20471.945386878688</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>27004</v>
+        <v>19875.675132891927</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -13519,43 +13461,43 @@
       </c>
       <c r="D8">
         <f>D2</f>
-        <v>27004</v>
+        <v>25920.517751770582</v>
       </c>
       <c r="E8">
         <f t="shared" ref="E8:M8" si="1">E2</f>
-        <v>27004</v>
+        <v>25177.910605727324</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>27004</v>
+        <v>24444.57340361876</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>27004</v>
+        <v>23732.59553749394</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>27004</v>
+        <v>23041.354890770817</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>27004</v>
+        <v>22370.247466767789</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>27004</v>
+        <v>21718.686860939597</v>
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>27004</v>
+        <v>21086.103748485046</v>
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>27004</v>
+        <v>20471.945386878688</v>
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
-        <v>27004</v>
+        <v>19875.675132891927</v>
       </c>
       <c r="N8">
         <v>0</v>

</xml_diff>